<commit_message>
ComponentAdd and BOM import
</commit_message>
<xml_diff>
--- a/src/lib/assets/ENG_CH_EAS.A_BC_EPA-003150_01_BOM.xlsx
+++ b/src/lib/assets/ENG_CH_EAS.A_BC_EPA-003150_01_BOM.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <fileSharing userName="Windows User" algorithmName="SHA-512" hashValue="RBRzeXxRCXCr6ddrS0d2otSUA9U48juc77Eo/PMuR3DajMGyYbr1KrnQGRwxr0AoP2Z2KnKgkCP1iiDmvm4NCA==" saltValue="Y0eSEilCzMzJLLyjDuuSrg==" spinCount="100000"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\New Quote Folder\EAS22314\4 BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\george\Documents\GitHub\EAMES\src\lib\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{4B3185CA-3692-486D-8D8C-1344797DA2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:10001_{C114BA6E-EE7F-4C7B-99DC-A06E39F8E150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1140" windowWidth="19200" windowHeight="15060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -3259,6 +3259,537 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="31" fillId="12" borderId="110" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="9" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="9" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="22" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3388,610 +3919,52 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="9" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="9" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="47" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="103" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="104" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="17" borderId="94" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4018,10 +3991,25 @@
     <xf numFmtId="0" fontId="18" fillId="10" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="108" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="109" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="28" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4034,6 +4022,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="17" borderId="102" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="102" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4045,47 +4039,53 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="47" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="48" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="103" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="100" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="104" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="99" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="12" borderId="110" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="92" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="96" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="97" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="93" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="27" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4760,313 +4760,313 @@
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="119" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="125" t="e">
+      <c r="B3" s="296" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="297"/>
+      <c r="D3" s="297"/>
+      <c r="E3" s="302" t="e">
         <f>RIGHT(BOM!#REF!,LEN(BOM!#REF!)-3)</f>
         <v>#REF!</v>
       </c>
-      <c r="F3" s="125"/>
-      <c r="G3" s="125"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="111" t="s">
+      <c r="F3" s="302"/>
+      <c r="G3" s="302"/>
+      <c r="H3" s="302"/>
+      <c r="I3" s="303"/>
+      <c r="J3" s="288" t="s">
         <v>143</v>
       </c>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
-      <c r="M3" s="111"/>
-      <c r="N3" s="111"/>
-      <c r="O3" s="111"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="105" t="str">
+      <c r="K3" s="288"/>
+      <c r="L3" s="288"/>
+      <c r="M3" s="288"/>
+      <c r="N3" s="288"/>
+      <c r="O3" s="288"/>
+      <c r="P3" s="289"/>
+      <c r="Q3" s="282" t="str">
         <f>"BOM Rev: " &amp; LOOKUP(2,1/(COUNTIF('Rev History'!$B$5:$B$19,"&gt;"&amp;'Rev History'!$B$5:$B$19&amp;"*")=0),'Rev History'!$B$5:$B$19)</f>
         <v>BOM Rev: A</v>
       </c>
-      <c r="R3" s="106"/>
-      <c r="S3" s="106"/>
-      <c r="T3" s="106"/>
-      <c r="U3" s="106"/>
-      <c r="V3" s="106"/>
-      <c r="W3" s="106"/>
-      <c r="X3" s="106"/>
-      <c r="Y3" s="107"/>
+      <c r="R3" s="283"/>
+      <c r="S3" s="283"/>
+      <c r="T3" s="283"/>
+      <c r="U3" s="283"/>
+      <c r="V3" s="283"/>
+      <c r="W3" s="283"/>
+      <c r="X3" s="283"/>
+      <c r="Y3" s="284"/>
       <c r="Z3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="121"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="127"/>
-      <c r="F4" s="127"/>
-      <c r="G4" s="127"/>
-      <c r="H4" s="127"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="113" t="e">
+      <c r="B4" s="298"/>
+      <c r="C4" s="299"/>
+      <c r="D4" s="299"/>
+      <c r="E4" s="304"/>
+      <c r="F4" s="304"/>
+      <c r="G4" s="304"/>
+      <c r="H4" s="304"/>
+      <c r="I4" s="305"/>
+      <c r="J4" s="290" t="e">
         <f>BOM!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="K4" s="113"/>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
-      <c r="N4" s="113"/>
-      <c r="O4" s="113"/>
-      <c r="P4" s="114"/>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="109"/>
-      <c r="S4" s="109"/>
-      <c r="T4" s="109"/>
-      <c r="U4" s="109"/>
-      <c r="V4" s="109"/>
-      <c r="W4" s="109"/>
-      <c r="X4" s="109"/>
-      <c r="Y4" s="110"/>
+      <c r="K4" s="290"/>
+      <c r="L4" s="290"/>
+      <c r="M4" s="290"/>
+      <c r="N4" s="290"/>
+      <c r="O4" s="290"/>
+      <c r="P4" s="291"/>
+      <c r="Q4" s="285"/>
+      <c r="R4" s="286"/>
+      <c r="S4" s="286"/>
+      <c r="T4" s="286"/>
+      <c r="U4" s="286"/>
+      <c r="V4" s="286"/>
+      <c r="W4" s="286"/>
+      <c r="X4" s="286"/>
+      <c r="Y4" s="287"/>
       <c r="Z4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122"/>
-      <c r="E5" s="127"/>
-      <c r="F5" s="127"/>
-      <c r="G5" s="127"/>
-      <c r="H5" s="127"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="115"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="96" t="s">
+      <c r="B5" s="298"/>
+      <c r="C5" s="299"/>
+      <c r="D5" s="299"/>
+      <c r="E5" s="304"/>
+      <c r="F5" s="304"/>
+      <c r="G5" s="304"/>
+      <c r="H5" s="304"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="292"/>
+      <c r="K5" s="292"/>
+      <c r="L5" s="292"/>
+      <c r="M5" s="292"/>
+      <c r="N5" s="292"/>
+      <c r="O5" s="292"/>
+      <c r="P5" s="293"/>
+      <c r="Q5" s="273" t="s">
         <v>179</v>
       </c>
-      <c r="R5" s="97"/>
-      <c r="S5" s="97"/>
-      <c r="T5" s="97"/>
-      <c r="U5" s="97"/>
-      <c r="V5" s="97"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="97"/>
-      <c r="Y5" s="98"/>
+      <c r="R5" s="274"/>
+      <c r="S5" s="274"/>
+      <c r="T5" s="274"/>
+      <c r="U5" s="274"/>
+      <c r="V5" s="274"/>
+      <c r="W5" s="274"/>
+      <c r="X5" s="274"/>
+      <c r="Y5" s="275"/>
       <c r="Z5" s="7"/>
     </row>
     <row r="6" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="127"/>
-      <c r="F6" s="127"/>
-      <c r="G6" s="127"/>
-      <c r="H6" s="127"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
-      <c r="M6" s="115"/>
-      <c r="N6" s="115"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="116"/>
-      <c r="Q6" s="99"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="100"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="100"/>
-      <c r="Y6" s="101"/>
+      <c r="B6" s="298"/>
+      <c r="C6" s="299"/>
+      <c r="D6" s="299"/>
+      <c r="E6" s="304"/>
+      <c r="F6" s="304"/>
+      <c r="G6" s="304"/>
+      <c r="H6" s="304"/>
+      <c r="I6" s="305"/>
+      <c r="J6" s="292"/>
+      <c r="K6" s="292"/>
+      <c r="L6" s="292"/>
+      <c r="M6" s="292"/>
+      <c r="N6" s="292"/>
+      <c r="O6" s="292"/>
+      <c r="P6" s="293"/>
+      <c r="Q6" s="276"/>
+      <c r="R6" s="277"/>
+      <c r="S6" s="277"/>
+      <c r="T6" s="277"/>
+      <c r="U6" s="277"/>
+      <c r="V6" s="277"/>
+      <c r="W6" s="277"/>
+      <c r="X6" s="277"/>
+      <c r="Y6" s="278"/>
       <c r="Z6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="124"/>
-      <c r="D7" s="124"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="129"/>
-      <c r="G7" s="129"/>
-      <c r="H7" s="129"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="117"/>
-      <c r="K7" s="117"/>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
-      <c r="N7" s="117"/>
-      <c r="O7" s="117"/>
-      <c r="P7" s="118"/>
-      <c r="Q7" s="102"/>
-      <c r="R7" s="103"/>
-      <c r="S7" s="103"/>
-      <c r="T7" s="103"/>
-      <c r="U7" s="103"/>
-      <c r="V7" s="103"/>
-      <c r="W7" s="103"/>
-      <c r="X7" s="103"/>
-      <c r="Y7" s="104"/>
+      <c r="B7" s="300"/>
+      <c r="C7" s="301"/>
+      <c r="D7" s="301"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="306"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="307"/>
+      <c r="J7" s="294"/>
+      <c r="K7" s="294"/>
+      <c r="L7" s="294"/>
+      <c r="M7" s="294"/>
+      <c r="N7" s="294"/>
+      <c r="O7" s="294"/>
+      <c r="P7" s="295"/>
+      <c r="Q7" s="279"/>
+      <c r="R7" s="280"/>
+      <c r="S7" s="280"/>
+      <c r="T7" s="280"/>
+      <c r="U7" s="280"/>
+      <c r="V7" s="280"/>
+      <c r="W7" s="280"/>
+      <c r="X7" s="280"/>
+      <c r="Y7" s="281"/>
       <c r="Z7" s="7"/>
     </row>
     <row r="8" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="151" t="s">
+      <c r="B8" s="248" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="152"/>
-      <c r="G8" s="152"/>
-      <c r="H8" s="152"/>
-      <c r="I8" s="152"/>
-      <c r="J8" s="149"/>
-      <c r="K8" s="149"/>
-      <c r="L8" s="150"/>
-      <c r="M8" s="148" t="s">
+      <c r="C8" s="249"/>
+      <c r="D8" s="249"/>
+      <c r="E8" s="249"/>
+      <c r="F8" s="249"/>
+      <c r="G8" s="249"/>
+      <c r="H8" s="249"/>
+      <c r="I8" s="249"/>
+      <c r="J8" s="246"/>
+      <c r="K8" s="246"/>
+      <c r="L8" s="247"/>
+      <c r="M8" s="245" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="149"/>
-      <c r="O8" s="149"/>
-      <c r="P8" s="149"/>
-      <c r="Q8" s="149"/>
-      <c r="R8" s="150"/>
-      <c r="S8" s="148" t="s">
+      <c r="N8" s="246"/>
+      <c r="O8" s="246"/>
+      <c r="P8" s="246"/>
+      <c r="Q8" s="246"/>
+      <c r="R8" s="247"/>
+      <c r="S8" s="245" t="s">
         <v>146</v>
       </c>
-      <c r="T8" s="149"/>
-      <c r="U8" s="149"/>
-      <c r="V8" s="149"/>
-      <c r="W8" s="149"/>
-      <c r="X8" s="149"/>
-      <c r="Y8" s="150"/>
+      <c r="T8" s="246"/>
+      <c r="U8" s="246"/>
+      <c r="V8" s="246"/>
+      <c r="W8" s="246"/>
+      <c r="X8" s="246"/>
+      <c r="Y8" s="247"/>
       <c r="Z8" s="7"/>
     </row>
     <row r="9" spans="1:26" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
-      <c r="B9" s="151"/>
-      <c r="C9" s="152"/>
-      <c r="D9" s="152"/>
-      <c r="E9" s="152"/>
-      <c r="F9" s="152"/>
-      <c r="G9" s="152"/>
-      <c r="H9" s="152"/>
-      <c r="I9" s="152"/>
-      <c r="J9" s="152"/>
-      <c r="K9" s="152"/>
-      <c r="L9" s="153"/>
-      <c r="M9" s="151"/>
-      <c r="N9" s="152"/>
-      <c r="O9" s="152"/>
-      <c r="P9" s="152"/>
-      <c r="Q9" s="152"/>
-      <c r="R9" s="153"/>
-      <c r="S9" s="151"/>
-      <c r="T9" s="152"/>
-      <c r="U9" s="152"/>
-      <c r="V9" s="152"/>
-      <c r="W9" s="152"/>
-      <c r="X9" s="152"/>
-      <c r="Y9" s="153"/>
+      <c r="B9" s="248"/>
+      <c r="C9" s="249"/>
+      <c r="D9" s="249"/>
+      <c r="E9" s="249"/>
+      <c r="F9" s="249"/>
+      <c r="G9" s="249"/>
+      <c r="H9" s="249"/>
+      <c r="I9" s="249"/>
+      <c r="J9" s="249"/>
+      <c r="K9" s="249"/>
+      <c r="L9" s="250"/>
+      <c r="M9" s="248"/>
+      <c r="N9" s="249"/>
+      <c r="O9" s="249"/>
+      <c r="P9" s="249"/>
+      <c r="Q9" s="249"/>
+      <c r="R9" s="250"/>
+      <c r="S9" s="248"/>
+      <c r="T9" s="249"/>
+      <c r="U9" s="249"/>
+      <c r="V9" s="249"/>
+      <c r="W9" s="249"/>
+      <c r="X9" s="249"/>
+      <c r="Y9" s="250"/>
       <c r="Z9" s="7"/>
     </row>
     <row r="10" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="154"/>
-      <c r="C10" s="155"/>
-      <c r="D10" s="155"/>
-      <c r="E10" s="155"/>
-      <c r="F10" s="155"/>
-      <c r="G10" s="155"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="155"/>
-      <c r="J10" s="155"/>
-      <c r="K10" s="155"/>
-      <c r="L10" s="156"/>
-      <c r="M10" s="154"/>
-      <c r="N10" s="155"/>
-      <c r="O10" s="155"/>
-      <c r="P10" s="155"/>
-      <c r="Q10" s="155"/>
-      <c r="R10" s="156"/>
-      <c r="S10" s="154"/>
-      <c r="T10" s="155"/>
-      <c r="U10" s="155"/>
-      <c r="V10" s="155"/>
-      <c r="W10" s="155"/>
-      <c r="X10" s="155"/>
-      <c r="Y10" s="156"/>
+      <c r="B10" s="255"/>
+      <c r="C10" s="251"/>
+      <c r="D10" s="251"/>
+      <c r="E10" s="251"/>
+      <c r="F10" s="251"/>
+      <c r="G10" s="251"/>
+      <c r="H10" s="251"/>
+      <c r="I10" s="251"/>
+      <c r="J10" s="251"/>
+      <c r="K10" s="251"/>
+      <c r="L10" s="252"/>
+      <c r="M10" s="255"/>
+      <c r="N10" s="251"/>
+      <c r="O10" s="251"/>
+      <c r="P10" s="251"/>
+      <c r="Q10" s="251"/>
+      <c r="R10" s="252"/>
+      <c r="S10" s="255"/>
+      <c r="T10" s="251"/>
+      <c r="U10" s="251"/>
+      <c r="V10" s="251"/>
+      <c r="W10" s="251"/>
+      <c r="X10" s="251"/>
+      <c r="Y10" s="252"/>
       <c r="Z10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
-      <c r="B11" s="135" t="s">
+      <c r="B11" s="312" t="s">
         <v>191</v>
       </c>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="131">
+      <c r="C11" s="313"/>
+      <c r="D11" s="313"/>
+      <c r="E11" s="313"/>
+      <c r="F11" s="313"/>
+      <c r="G11" s="308">
         <v>45169</v>
       </c>
-      <c r="H11" s="131"/>
-      <c r="I11" s="131"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="131"/>
-      <c r="L11" s="132"/>
-      <c r="M11" s="139" t="s">
+      <c r="H11" s="308"/>
+      <c r="I11" s="308"/>
+      <c r="J11" s="308"/>
+      <c r="K11" s="308"/>
+      <c r="L11" s="309"/>
+      <c r="M11" s="128" t="s">
         <v>144</v>
       </c>
-      <c r="N11" s="140"/>
-      <c r="O11" s="141"/>
-      <c r="P11" s="139" t="s">
+      <c r="N11" s="129"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="128" t="s">
         <v>145</v>
       </c>
-      <c r="Q11" s="140"/>
-      <c r="R11" s="141"/>
-      <c r="S11" s="139" t="s">
+      <c r="Q11" s="129"/>
+      <c r="R11" s="130"/>
+      <c r="S11" s="128" t="s">
         <v>147</v>
       </c>
-      <c r="T11" s="140"/>
-      <c r="U11" s="140"/>
-      <c r="V11" s="140"/>
-      <c r="W11" s="140"/>
-      <c r="X11" s="140"/>
-      <c r="Y11" s="141"/>
+      <c r="T11" s="129"/>
+      <c r="U11" s="129"/>
+      <c r="V11" s="129"/>
+      <c r="W11" s="129"/>
+      <c r="X11" s="129"/>
+      <c r="Y11" s="130"/>
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="137"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="142"/>
-      <c r="N12" s="143"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="142"/>
-      <c r="Q12" s="143"/>
-      <c r="R12" s="144"/>
-      <c r="S12" s="145"/>
-      <c r="T12" s="146"/>
-      <c r="U12" s="146"/>
-      <c r="V12" s="146"/>
-      <c r="W12" s="146"/>
-      <c r="X12" s="146"/>
-      <c r="Y12" s="147"/>
+      <c r="B12" s="314"/>
+      <c r="C12" s="315"/>
+      <c r="D12" s="315"/>
+      <c r="E12" s="315"/>
+      <c r="F12" s="315"/>
+      <c r="G12" s="310"/>
+      <c r="H12" s="310"/>
+      <c r="I12" s="310"/>
+      <c r="J12" s="310"/>
+      <c r="K12" s="310"/>
+      <c r="L12" s="311"/>
+      <c r="M12" s="131"/>
+      <c r="N12" s="132"/>
+      <c r="O12" s="133"/>
+      <c r="P12" s="131"/>
+      <c r="Q12" s="132"/>
+      <c r="R12" s="133"/>
+      <c r="S12" s="170"/>
+      <c r="T12" s="171"/>
+      <c r="U12" s="171"/>
+      <c r="V12" s="171"/>
+      <c r="W12" s="171"/>
+      <c r="X12" s="171"/>
+      <c r="Y12" s="172"/>
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5082,97 +5082,97 @@
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
       <c r="L13" s="11"/>
-      <c r="M13" s="165"/>
-      <c r="N13" s="166"/>
-      <c r="O13" s="167"/>
-      <c r="P13" s="165"/>
-      <c r="Q13" s="166"/>
-      <c r="R13" s="166"/>
-      <c r="S13" s="239" t="s">
+      <c r="M13" s="158"/>
+      <c r="N13" s="152"/>
+      <c r="O13" s="153"/>
+      <c r="P13" s="158"/>
+      <c r="Q13" s="152"/>
+      <c r="R13" s="152"/>
+      <c r="S13" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="T13" s="241"/>
-      <c r="U13" s="311" t="e">
+      <c r="T13" s="102"/>
+      <c r="U13" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S13,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V13" s="312"/>
-      <c r="W13" s="239" t="s">
+      <c r="V13" s="98"/>
+      <c r="W13" s="101" t="s">
         <v>186</v>
       </c>
-      <c r="X13" s="240"/>
-      <c r="Y13" s="241"/>
+      <c r="X13" s="105"/>
+      <c r="Y13" s="102"/>
       <c r="Z13" s="7"/>
     </row>
     <row r="14" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="237" t="s">
         <v>151</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="159"/>
-      <c r="E14" s="179" t="s">
+      <c r="C14" s="238"/>
+      <c r="D14" s="239"/>
+      <c r="E14" s="259" t="s">
         <v>229</v>
       </c>
-      <c r="F14" s="180"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="181"/>
+      <c r="F14" s="260"/>
+      <c r="G14" s="260"/>
+      <c r="H14" s="261"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="185"/>
-      <c r="K14" s="174">
+      <c r="J14" s="265"/>
+      <c r="K14" s="253">
         <f>COUNTIF(Calculations!G:G,1)</f>
         <v>0</v>
       </c>
       <c r="L14" s="15"/>
-      <c r="M14" s="168"/>
-      <c r="N14" s="169"/>
-      <c r="O14" s="170"/>
-      <c r="P14" s="168"/>
-      <c r="Q14" s="169"/>
-      <c r="R14" s="169"/>
-      <c r="S14" s="242"/>
-      <c r="T14" s="244"/>
-      <c r="U14" s="313"/>
-      <c r="V14" s="314"/>
-      <c r="W14" s="242"/>
-      <c r="X14" s="243"/>
-      <c r="Y14" s="244"/>
+      <c r="M14" s="159"/>
+      <c r="N14" s="154"/>
+      <c r="O14" s="155"/>
+      <c r="P14" s="159"/>
+      <c r="Q14" s="154"/>
+      <c r="R14" s="154"/>
+      <c r="S14" s="103"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="99"/>
+      <c r="V14" s="100"/>
+      <c r="W14" s="103"/>
+      <c r="X14" s="106"/>
+      <c r="Y14" s="104"/>
       <c r="Z14" s="7"/>
     </row>
     <row r="15" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="160"/>
-      <c r="C15" s="161"/>
-      <c r="D15" s="162"/>
-      <c r="E15" s="182"/>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183"/>
-      <c r="H15" s="184"/>
+      <c r="B15" s="240"/>
+      <c r="C15" s="241"/>
+      <c r="D15" s="242"/>
+      <c r="E15" s="262"/>
+      <c r="F15" s="263"/>
+      <c r="G15" s="263"/>
+      <c r="H15" s="264"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="186"/>
-      <c r="K15" s="175"/>
+      <c r="J15" s="266"/>
+      <c r="K15" s="254"/>
       <c r="L15" s="15"/>
-      <c r="M15" s="168"/>
-      <c r="N15" s="169"/>
-      <c r="O15" s="170"/>
-      <c r="P15" s="168"/>
-      <c r="Q15" s="169"/>
-      <c r="R15" s="170"/>
-      <c r="S15" s="239" t="s">
+      <c r="M15" s="159"/>
+      <c r="N15" s="154"/>
+      <c r="O15" s="155"/>
+      <c r="P15" s="159"/>
+      <c r="Q15" s="154"/>
+      <c r="R15" s="155"/>
+      <c r="S15" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="T15" s="241"/>
-      <c r="U15" s="311" t="e">
+      <c r="T15" s="102"/>
+      <c r="U15" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S15,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V15" s="312"/>
-      <c r="W15" s="245">
+      <c r="V15" s="98"/>
+      <c r="W15" s="107">
         <f>SUMIF(Calculations!M:M,"&gt;0",Calculations!M:M)</f>
         <v>0</v>
       </c>
-      <c r="X15" s="246"/>
-      <c r="Y15" s="247"/>
+      <c r="X15" s="108"/>
+      <c r="Y15" s="109"/>
       <c r="Z15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5183,103 +5183,103 @@
       <c r="G16" s="10"/>
       <c r="H16" s="14"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="187"/>
-      <c r="K16" s="174">
+      <c r="J16" s="267"/>
+      <c r="K16" s="253">
         <f>COUNTIF(Calculations!L:L,1)</f>
         <v>0</v>
       </c>
       <c r="L16" s="15"/>
-      <c r="M16" s="168"/>
-      <c r="N16" s="169"/>
-      <c r="O16" s="170"/>
-      <c r="P16" s="168"/>
-      <c r="Q16" s="169"/>
-      <c r="R16" s="170"/>
-      <c r="S16" s="242"/>
-      <c r="T16" s="244"/>
-      <c r="U16" s="313"/>
-      <c r="V16" s="314"/>
-      <c r="W16" s="248"/>
-      <c r="X16" s="249"/>
-      <c r="Y16" s="250"/>
+      <c r="M16" s="159"/>
+      <c r="N16" s="154"/>
+      <c r="O16" s="155"/>
+      <c r="P16" s="159"/>
+      <c r="Q16" s="154"/>
+      <c r="R16" s="155"/>
+      <c r="S16" s="103"/>
+      <c r="T16" s="104"/>
+      <c r="U16" s="99"/>
+      <c r="V16" s="100"/>
+      <c r="W16" s="110"/>
+      <c r="X16" s="111"/>
+      <c r="Y16" s="112"/>
       <c r="Z16" s="7"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="237" t="s">
         <v>150</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="159"/>
-      <c r="E17" s="262" t="e">
+      <c r="C17" s="238"/>
+      <c r="D17" s="239"/>
+      <c r="E17" s="179" t="e">
         <f>BOM!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F17" s="163" t="s">
+      <c r="F17" s="243" t="s">
         <v>152</v>
       </c>
-      <c r="G17" s="159"/>
-      <c r="H17" s="270" t="e">
+      <c r="G17" s="239"/>
+      <c r="H17" s="187" t="e">
         <f>COUNTIF(BOM!#REF!,"&gt;=0")</f>
         <v>#REF!</v>
       </c>
       <c r="I17" s="15"/>
-      <c r="J17" s="188"/>
-      <c r="K17" s="175"/>
+      <c r="J17" s="268"/>
+      <c r="K17" s="254"/>
       <c r="L17" s="15"/>
-      <c r="M17" s="171"/>
-      <c r="N17" s="172"/>
-      <c r="O17" s="173"/>
-      <c r="P17" s="171"/>
-      <c r="Q17" s="172"/>
-      <c r="R17" s="173"/>
-      <c r="S17" s="239" t="s">
+      <c r="M17" s="160"/>
+      <c r="N17" s="156"/>
+      <c r="O17" s="157"/>
+      <c r="P17" s="160"/>
+      <c r="Q17" s="156"/>
+      <c r="R17" s="157"/>
+      <c r="S17" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="T17" s="241"/>
-      <c r="U17" s="311" t="e">
+      <c r="T17" s="102"/>
+      <c r="U17" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S17,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V17" s="312"/>
-      <c r="W17" s="251"/>
-      <c r="X17" s="252"/>
-      <c r="Y17" s="253"/>
+      <c r="V17" s="98"/>
+      <c r="W17" s="113"/>
+      <c r="X17" s="114"/>
+      <c r="Y17" s="115"/>
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="160"/>
-      <c r="C18" s="161"/>
-      <c r="D18" s="162"/>
-      <c r="E18" s="263"/>
-      <c r="F18" s="164"/>
-      <c r="G18" s="162"/>
-      <c r="H18" s="271"/>
+      <c r="B18" s="240"/>
+      <c r="C18" s="241"/>
+      <c r="D18" s="242"/>
+      <c r="E18" s="180"/>
+      <c r="F18" s="244"/>
+      <c r="G18" s="242"/>
+      <c r="H18" s="188"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="189"/>
-      <c r="K18" s="174">
+      <c r="J18" s="269"/>
+      <c r="K18" s="253">
         <f>COUNTIF(Calculations!F:F,1)</f>
         <v>0</v>
       </c>
       <c r="L18" s="15"/>
-      <c r="M18" s="139" t="s">
+      <c r="M18" s="128" t="s">
         <v>148</v>
       </c>
-      <c r="N18" s="140"/>
-      <c r="O18" s="140"/>
-      <c r="P18" s="140"/>
-      <c r="Q18" s="140"/>
-      <c r="R18" s="141"/>
-      <c r="S18" s="242"/>
-      <c r="T18" s="244"/>
-      <c r="U18" s="313"/>
-      <c r="V18" s="314"/>
-      <c r="W18" s="239" t="s">
+      <c r="N18" s="129"/>
+      <c r="O18" s="129"/>
+      <c r="P18" s="129"/>
+      <c r="Q18" s="129"/>
+      <c r="R18" s="130"/>
+      <c r="S18" s="103"/>
+      <c r="T18" s="104"/>
+      <c r="U18" s="99"/>
+      <c r="V18" s="100"/>
+      <c r="W18" s="101" t="s">
         <v>225</v>
       </c>
-      <c r="X18" s="240"/>
-      <c r="Y18" s="241"/>
+      <c r="X18" s="105"/>
+      <c r="Y18" s="102"/>
       <c r="Z18" s="7"/>
     </row>
     <row r="19" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5290,102 +5290,102 @@
       <c r="G19" s="5"/>
       <c r="H19" s="14"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="190"/>
-      <c r="K19" s="175"/>
+      <c r="J19" s="270"/>
+      <c r="K19" s="254"/>
       <c r="L19" s="15"/>
-      <c r="M19" s="145"/>
-      <c r="N19" s="146"/>
-      <c r="O19" s="146"/>
-      <c r="P19" s="146"/>
-      <c r="Q19" s="146"/>
-      <c r="R19" s="147"/>
-      <c r="S19" s="239" t="s">
+      <c r="M19" s="170"/>
+      <c r="N19" s="171"/>
+      <c r="O19" s="171"/>
+      <c r="P19" s="171"/>
+      <c r="Q19" s="171"/>
+      <c r="R19" s="172"/>
+      <c r="S19" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="T19" s="241"/>
-      <c r="U19" s="311" t="e">
+      <c r="T19" s="102"/>
+      <c r="U19" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S19,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V19" s="312"/>
-      <c r="W19" s="242"/>
-      <c r="X19" s="243"/>
-      <c r="Y19" s="244"/>
+      <c r="V19" s="98"/>
+      <c r="W19" s="103"/>
+      <c r="X19" s="106"/>
+      <c r="Y19" s="104"/>
       <c r="Z19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="157" t="s">
+      <c r="B20" s="237" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="158"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="264" t="e">
+      <c r="C20" s="238"/>
+      <c r="D20" s="239"/>
+      <c r="E20" s="181" t="e">
         <f>BOM!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="F20" s="265"/>
-      <c r="G20" s="265"/>
-      <c r="H20" s="266"/>
+      <c r="F20" s="182"/>
+      <c r="G20" s="182"/>
+      <c r="H20" s="183"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="191"/>
-      <c r="K20" s="174">
+      <c r="J20" s="271"/>
+      <c r="K20" s="253">
         <f>COUNTIF(Calculations!J:J,1)</f>
         <v>0</v>
       </c>
       <c r="L20" s="15"/>
-      <c r="M20" s="193" t="s">
+      <c r="M20" s="122" t="s">
         <v>272</v>
       </c>
-      <c r="N20" s="194"/>
-      <c r="O20" s="195"/>
-      <c r="P20" s="193" t="s">
+      <c r="N20" s="123"/>
+      <c r="O20" s="124"/>
+      <c r="P20" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="Q20" s="194"/>
-      <c r="R20" s="195"/>
-      <c r="S20" s="243"/>
-      <c r="T20" s="244"/>
-      <c r="U20" s="313"/>
-      <c r="V20" s="314"/>
-      <c r="W20" s="245">
-        <v>0</v>
-      </c>
-      <c r="X20" s="246"/>
-      <c r="Y20" s="247"/>
+      <c r="Q20" s="123"/>
+      <c r="R20" s="124"/>
+      <c r="S20" s="106"/>
+      <c r="T20" s="104"/>
+      <c r="U20" s="99"/>
+      <c r="V20" s="100"/>
+      <c r="W20" s="107">
+        <v>0</v>
+      </c>
+      <c r="X20" s="108"/>
+      <c r="Y20" s="109"/>
       <c r="Z20" s="7"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="160"/>
-      <c r="C21" s="161"/>
-      <c r="D21" s="162"/>
-      <c r="E21" s="267"/>
-      <c r="F21" s="268"/>
-      <c r="G21" s="268"/>
-      <c r="H21" s="269"/>
+      <c r="B21" s="240"/>
+      <c r="C21" s="241"/>
+      <c r="D21" s="242"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="185"/>
+      <c r="G21" s="185"/>
+      <c r="H21" s="186"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="192"/>
-      <c r="K21" s="175"/>
+      <c r="J21" s="272"/>
+      <c r="K21" s="254"/>
       <c r="L21" s="15"/>
-      <c r="M21" s="196"/>
-      <c r="N21" s="197"/>
-      <c r="O21" s="198"/>
-      <c r="P21" s="196"/>
-      <c r="Q21" s="197"/>
-      <c r="R21" s="198"/>
-      <c r="S21" s="240" t="s">
+      <c r="M21" s="125"/>
+      <c r="N21" s="126"/>
+      <c r="O21" s="127"/>
+      <c r="P21" s="125"/>
+      <c r="Q21" s="126"/>
+      <c r="R21" s="127"/>
+      <c r="S21" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="T21" s="241"/>
-      <c r="U21" s="311" t="e">
+      <c r="T21" s="102"/>
+      <c r="U21" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S21,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V21" s="312"/>
-      <c r="W21" s="248"/>
-      <c r="X21" s="249"/>
-      <c r="Y21" s="250"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="110"/>
+      <c r="X21" s="111"/>
+      <c r="Y21" s="112"/>
       <c r="Z21" s="7"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5401,275 +5401,275 @@
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="6"/>
-      <c r="M22" s="218" t="s">
+      <c r="M22" s="231" t="s">
         <v>273</v>
       </c>
-      <c r="N22" s="202">
+      <c r="N22" s="219">
         <f>COUNTIF(Calculations!D:D,0)</f>
         <v>0</v>
       </c>
-      <c r="O22" s="205" t="e">
+      <c r="O22" s="222" t="e">
         <f>$N$22/$H$17</f>
         <v>#REF!</v>
       </c>
-      <c r="P22" s="199" t="s">
+      <c r="P22" s="234" t="s">
         <v>274</v>
       </c>
-      <c r="Q22" s="202">
+      <c r="Q22" s="219">
         <f>COUNTIF(Calculations!A:A,2)</f>
         <v>0</v>
       </c>
-      <c r="R22" s="205" t="e">
+      <c r="R22" s="222" t="e">
         <f>$Q$22/$H$17</f>
         <v>#REF!</v>
       </c>
-      <c r="S22" s="243"/>
-      <c r="T22" s="244"/>
-      <c r="U22" s="313"/>
-      <c r="V22" s="314"/>
-      <c r="W22" s="251"/>
-      <c r="X22" s="252"/>
-      <c r="Y22" s="253"/>
+      <c r="S22" s="106"/>
+      <c r="T22" s="104"/>
+      <c r="U22" s="99"/>
+      <c r="V22" s="100"/>
+      <c r="W22" s="113"/>
+      <c r="X22" s="114"/>
+      <c r="Y22" s="115"/>
       <c r="Z22" s="7"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
       <c r="B23" s="16"/>
-      <c r="C23" s="272" t="s">
+      <c r="C23" s="189" t="s">
         <v>161</v>
       </c>
-      <c r="D23" s="273"/>
-      <c r="E23" s="274"/>
-      <c r="F23" s="305" t="s">
+      <c r="D23" s="190"/>
+      <c r="E23" s="191"/>
+      <c r="F23" s="164" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="306"/>
-      <c r="H23" s="302" t="s">
+      <c r="G23" s="165"/>
+      <c r="H23" s="161" t="s">
         <v>173</v>
       </c>
-      <c r="I23" s="303"/>
-      <c r="J23" s="303"/>
-      <c r="K23" s="304"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="162"/>
+      <c r="K23" s="163"/>
       <c r="L23" s="15"/>
-      <c r="M23" s="219"/>
-      <c r="N23" s="203"/>
-      <c r="O23" s="206"/>
-      <c r="P23" s="200"/>
-      <c r="Q23" s="203"/>
-      <c r="R23" s="206"/>
-      <c r="S23" s="240" t="s">
+      <c r="M23" s="232"/>
+      <c r="N23" s="220"/>
+      <c r="O23" s="223"/>
+      <c r="P23" s="235"/>
+      <c r="Q23" s="220"/>
+      <c r="R23" s="223"/>
+      <c r="S23" s="105" t="s">
         <v>221</v>
       </c>
-      <c r="T23" s="241"/>
-      <c r="U23" s="311" t="e">
+      <c r="T23" s="102"/>
+      <c r="U23" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S23,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V23" s="312"/>
-      <c r="W23" s="239" t="s">
+      <c r="V23" s="98"/>
+      <c r="W23" s="101" t="s">
         <v>226</v>
       </c>
-      <c r="X23" s="240"/>
-      <c r="Y23" s="241"/>
+      <c r="X23" s="105"/>
+      <c r="Y23" s="102"/>
       <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
       <c r="B24" s="16"/>
-      <c r="C24" s="275" t="s">
+      <c r="C24" s="192" t="s">
         <v>162</v>
       </c>
-      <c r="D24" s="276"/>
-      <c r="E24" s="277"/>
-      <c r="F24" s="307" t="s">
+      <c r="D24" s="193"/>
+      <c r="E24" s="194"/>
+      <c r="F24" s="166" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="308"/>
-      <c r="H24" s="212" t="s">
+      <c r="G24" s="167"/>
+      <c r="H24" s="225" t="s">
         <v>174</v>
       </c>
-      <c r="I24" s="213"/>
-      <c r="J24" s="213"/>
-      <c r="K24" s="214"/>
+      <c r="I24" s="226"/>
+      <c r="J24" s="226"/>
+      <c r="K24" s="227"/>
       <c r="L24" s="15"/>
-      <c r="M24" s="219"/>
-      <c r="N24" s="203"/>
-      <c r="O24" s="206"/>
-      <c r="P24" s="200"/>
-      <c r="Q24" s="203"/>
-      <c r="R24" s="206"/>
-      <c r="S24" s="243"/>
-      <c r="T24" s="244"/>
-      <c r="U24" s="313"/>
-      <c r="V24" s="314"/>
-      <c r="W24" s="242"/>
-      <c r="X24" s="243"/>
-      <c r="Y24" s="244"/>
+      <c r="M24" s="232"/>
+      <c r="N24" s="220"/>
+      <c r="O24" s="223"/>
+      <c r="P24" s="235"/>
+      <c r="Q24" s="220"/>
+      <c r="R24" s="223"/>
+      <c r="S24" s="106"/>
+      <c r="T24" s="104"/>
+      <c r="U24" s="99"/>
+      <c r="V24" s="100"/>
+      <c r="W24" s="103"/>
+      <c r="X24" s="106"/>
+      <c r="Y24" s="104"/>
       <c r="Z24" s="7"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
       <c r="B25" s="16"/>
-      <c r="C25" s="278" t="s">
+      <c r="C25" s="195" t="s">
         <v>163</v>
       </c>
-      <c r="D25" s="279"/>
-      <c r="E25" s="280"/>
-      <c r="F25" s="307" t="s">
+      <c r="D25" s="196"/>
+      <c r="E25" s="197"/>
+      <c r="F25" s="166" t="s">
         <v>169</v>
       </c>
-      <c r="G25" s="308"/>
-      <c r="H25" s="212" t="s">
+      <c r="G25" s="167"/>
+      <c r="H25" s="225" t="s">
         <v>175</v>
       </c>
-      <c r="I25" s="213"/>
-      <c r="J25" s="213"/>
-      <c r="K25" s="214"/>
+      <c r="I25" s="226"/>
+      <c r="J25" s="226"/>
+      <c r="K25" s="227"/>
       <c r="L25" s="15"/>
-      <c r="M25" s="220"/>
-      <c r="N25" s="204"/>
-      <c r="O25" s="207"/>
-      <c r="P25" s="201"/>
-      <c r="Q25" s="204"/>
-      <c r="R25" s="207"/>
-      <c r="S25" s="240" t="s">
+      <c r="M25" s="233"/>
+      <c r="N25" s="221"/>
+      <c r="O25" s="224"/>
+      <c r="P25" s="236"/>
+      <c r="Q25" s="221"/>
+      <c r="R25" s="224"/>
+      <c r="S25" s="105" t="s">
         <v>222</v>
       </c>
-      <c r="T25" s="241"/>
-      <c r="U25" s="311" t="e">
+      <c r="T25" s="102"/>
+      <c r="U25" s="97" t="e">
         <f>SUMIF(BOM!#REF!,$S25,BOM!#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="V25" s="312"/>
-      <c r="W25" s="230" t="str">
+      <c r="V25" s="98"/>
+      <c r="W25" s="210" t="str">
         <f>IFERROR(($W$15/$S$35),"0")</f>
         <v>0</v>
       </c>
-      <c r="X25" s="231"/>
-      <c r="Y25" s="232"/>
+      <c r="X25" s="211"/>
+      <c r="Y25" s="212"/>
       <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6"/>
       <c r="B26" s="16"/>
-      <c r="C26" s="281" t="s">
+      <c r="C26" s="198" t="s">
         <v>164</v>
       </c>
-      <c r="D26" s="282"/>
-      <c r="E26" s="283"/>
-      <c r="F26" s="307" t="s">
+      <c r="D26" s="199"/>
+      <c r="E26" s="200"/>
+      <c r="F26" s="166" t="s">
         <v>170</v>
       </c>
-      <c r="G26" s="308"/>
-      <c r="H26" s="212" t="s">
+      <c r="G26" s="167"/>
+      <c r="H26" s="225" t="s">
         <v>176</v>
       </c>
-      <c r="I26" s="213"/>
-      <c r="J26" s="213"/>
-      <c r="K26" s="214"/>
+      <c r="I26" s="226"/>
+      <c r="J26" s="226"/>
+      <c r="K26" s="227"/>
       <c r="L26" s="15"/>
-      <c r="M26" s="199" t="s">
+      <c r="M26" s="234" t="s">
         <v>185</v>
       </c>
-      <c r="N26" s="202">
+      <c r="N26" s="219">
         <f>COUNTIF(Calculations!H:H,1)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="205">
+      <c r="O26" s="222">
         <f>IFERROR(N26/N22,0)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="218" t="s">
+      <c r="P26" s="231" t="s">
         <v>275</v>
       </c>
-      <c r="Q26" s="202">
+      <c r="Q26" s="219">
         <f>COUNTIF(Calculations!A:A,3)</f>
         <v>0</v>
       </c>
-      <c r="R26" s="205" t="e">
+      <c r="R26" s="222" t="e">
         <f>$Q$26/$H$17</f>
         <v>#REF!</v>
       </c>
-      <c r="S26" s="242"/>
-      <c r="T26" s="244"/>
-      <c r="U26" s="313"/>
-      <c r="V26" s="314"/>
-      <c r="W26" s="233"/>
-      <c r="X26" s="234"/>
-      <c r="Y26" s="235"/>
+      <c r="S26" s="103"/>
+      <c r="T26" s="104"/>
+      <c r="U26" s="99"/>
+      <c r="V26" s="100"/>
+      <c r="W26" s="213"/>
+      <c r="X26" s="214"/>
+      <c r="Y26" s="215"/>
       <c r="Z26" s="7"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="16"/>
-      <c r="C27" s="299" t="s">
+      <c r="C27" s="149" t="s">
         <v>165</v>
       </c>
-      <c r="D27" s="300"/>
-      <c r="E27" s="301"/>
-      <c r="F27" s="307" t="s">
+      <c r="D27" s="150"/>
+      <c r="E27" s="151"/>
+      <c r="F27" s="166" t="s">
         <v>171</v>
       </c>
-      <c r="G27" s="308"/>
-      <c r="H27" s="212" t="s">
+      <c r="G27" s="167"/>
+      <c r="H27" s="225" t="s">
         <v>177</v>
       </c>
-      <c r="I27" s="213"/>
-      <c r="J27" s="213"/>
-      <c r="K27" s="214"/>
+      <c r="I27" s="226"/>
+      <c r="J27" s="226"/>
+      <c r="K27" s="227"/>
       <c r="L27" s="15"/>
-      <c r="M27" s="200"/>
-      <c r="N27" s="203"/>
-      <c r="O27" s="206"/>
-      <c r="P27" s="219"/>
-      <c r="Q27" s="203"/>
-      <c r="R27" s="206"/>
-      <c r="S27" s="239" t="s">
+      <c r="M27" s="235"/>
+      <c r="N27" s="220"/>
+      <c r="O27" s="223"/>
+      <c r="P27" s="232"/>
+      <c r="Q27" s="220"/>
+      <c r="R27" s="223"/>
+      <c r="S27" s="101" t="s">
         <v>223</v>
       </c>
-      <c r="T27" s="241"/>
-      <c r="U27" s="311" t="e">
+      <c r="T27" s="102"/>
+      <c r="U27" s="97" t="e">
         <f>SUM(BOM!#REF!)-SUM(Overview!U13:V26)</f>
         <v>#REF!</v>
       </c>
-      <c r="V27" s="312"/>
-      <c r="W27" s="233"/>
-      <c r="X27" s="234"/>
-      <c r="Y27" s="235"/>
+      <c r="V27" s="98"/>
+      <c r="W27" s="213"/>
+      <c r="X27" s="214"/>
+      <c r="Y27" s="215"/>
       <c r="Z27" s="7"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6"/>
       <c r="B28" s="16"/>
-      <c r="C28" s="176" t="s">
+      <c r="C28" s="256" t="s">
         <v>166</v>
       </c>
-      <c r="D28" s="177"/>
-      <c r="E28" s="178"/>
-      <c r="F28" s="309" t="s">
+      <c r="D28" s="257"/>
+      <c r="E28" s="258"/>
+      <c r="F28" s="168" t="s">
         <v>172</v>
       </c>
-      <c r="G28" s="310"/>
-      <c r="H28" s="215" t="s">
+      <c r="G28" s="169"/>
+      <c r="H28" s="228" t="s">
         <v>178</v>
       </c>
-      <c r="I28" s="216"/>
-      <c r="J28" s="216"/>
-      <c r="K28" s="217"/>
+      <c r="I28" s="229"/>
+      <c r="J28" s="229"/>
+      <c r="K28" s="230"/>
       <c r="L28" s="15"/>
-      <c r="M28" s="200"/>
-      <c r="N28" s="203"/>
-      <c r="O28" s="206"/>
-      <c r="P28" s="219"/>
-      <c r="Q28" s="203"/>
-      <c r="R28" s="206"/>
-      <c r="S28" s="242"/>
-      <c r="T28" s="244"/>
-      <c r="U28" s="313"/>
-      <c r="V28" s="314"/>
-      <c r="W28" s="233"/>
-      <c r="X28" s="234"/>
-      <c r="Y28" s="235"/>
+      <c r="M28" s="235"/>
+      <c r="N28" s="220"/>
+      <c r="O28" s="223"/>
+      <c r="P28" s="232"/>
+      <c r="Q28" s="220"/>
+      <c r="R28" s="223"/>
+      <c r="S28" s="103"/>
+      <c r="T28" s="104"/>
+      <c r="U28" s="99"/>
+      <c r="V28" s="100"/>
+      <c r="W28" s="213"/>
+      <c r="X28" s="214"/>
+      <c r="Y28" s="215"/>
       <c r="Z28" s="7"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5685,534 +5685,534 @@
       <c r="J29" s="14"/>
       <c r="K29" s="14"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="201"/>
-      <c r="N29" s="204"/>
-      <c r="O29" s="207"/>
-      <c r="P29" s="220"/>
-      <c r="Q29" s="204"/>
-      <c r="R29" s="207"/>
-      <c r="S29" s="239" t="s">
+      <c r="M29" s="236"/>
+      <c r="N29" s="221"/>
+      <c r="O29" s="224"/>
+      <c r="P29" s="233"/>
+      <c r="Q29" s="221"/>
+      <c r="R29" s="224"/>
+      <c r="S29" s="101" t="s">
         <v>224</v>
       </c>
-      <c r="T29" s="241"/>
-      <c r="U29" s="311">
-        <v>0</v>
-      </c>
-      <c r="V29" s="312"/>
-      <c r="W29" s="233"/>
-      <c r="X29" s="234"/>
-      <c r="Y29" s="235"/>
+      <c r="T29" s="102"/>
+      <c r="U29" s="97">
+        <v>0</v>
+      </c>
+      <c r="V29" s="98"/>
+      <c r="W29" s="213"/>
+      <c r="X29" s="214"/>
+      <c r="Y29" s="215"/>
       <c r="Z29" s="7"/>
     </row>
     <row r="30" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6"/>
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="245" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="149"/>
-      <c r="D30" s="149"/>
-      <c r="E30" s="149"/>
-      <c r="F30" s="149"/>
-      <c r="G30" s="149"/>
-      <c r="H30" s="149"/>
-      <c r="I30" s="149"/>
-      <c r="J30" s="149"/>
-      <c r="K30" s="149"/>
-      <c r="L30" s="150"/>
-      <c r="M30" s="151" t="s">
+      <c r="C30" s="246"/>
+      <c r="D30" s="246"/>
+      <c r="E30" s="246"/>
+      <c r="F30" s="246"/>
+      <c r="G30" s="246"/>
+      <c r="H30" s="246"/>
+      <c r="I30" s="246"/>
+      <c r="J30" s="246"/>
+      <c r="K30" s="246"/>
+      <c r="L30" s="247"/>
+      <c r="M30" s="248" t="s">
         <v>156</v>
       </c>
-      <c r="N30" s="152"/>
-      <c r="O30" s="152"/>
-      <c r="P30" s="152"/>
-      <c r="Q30" s="152"/>
-      <c r="R30" s="150"/>
-      <c r="S30" s="242"/>
-      <c r="T30" s="244"/>
-      <c r="U30" s="313"/>
-      <c r="V30" s="314"/>
-      <c r="W30" s="236"/>
-      <c r="X30" s="237"/>
-      <c r="Y30" s="238"/>
+      <c r="N30" s="249"/>
+      <c r="O30" s="249"/>
+      <c r="P30" s="249"/>
+      <c r="Q30" s="249"/>
+      <c r="R30" s="247"/>
+      <c r="S30" s="103"/>
+      <c r="T30" s="104"/>
+      <c r="U30" s="99"/>
+      <c r="V30" s="100"/>
+      <c r="W30" s="216"/>
+      <c r="X30" s="217"/>
+      <c r="Y30" s="218"/>
       <c r="Z30" s="7"/>
     </row>
     <row r="31" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="152"/>
-      <c r="D31" s="152"/>
-      <c r="E31" s="152"/>
-      <c r="F31" s="152"/>
-      <c r="G31" s="152"/>
-      <c r="H31" s="152"/>
-      <c r="I31" s="152"/>
-      <c r="J31" s="152"/>
-      <c r="K31" s="152"/>
-      <c r="L31" s="153"/>
-      <c r="M31" s="151"/>
-      <c r="N31" s="152"/>
-      <c r="O31" s="152"/>
-      <c r="P31" s="152"/>
-      <c r="Q31" s="152"/>
-      <c r="R31" s="152"/>
-      <c r="S31" s="139" t="s">
+      <c r="B31" s="248"/>
+      <c r="C31" s="249"/>
+      <c r="D31" s="249"/>
+      <c r="E31" s="249"/>
+      <c r="F31" s="249"/>
+      <c r="G31" s="249"/>
+      <c r="H31" s="249"/>
+      <c r="I31" s="249"/>
+      <c r="J31" s="249"/>
+      <c r="K31" s="249"/>
+      <c r="L31" s="250"/>
+      <c r="M31" s="248"/>
+      <c r="N31" s="249"/>
+      <c r="O31" s="249"/>
+      <c r="P31" s="249"/>
+      <c r="Q31" s="249"/>
+      <c r="R31" s="249"/>
+      <c r="S31" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="T31" s="140"/>
-      <c r="U31" s="140"/>
-      <c r="V31" s="140"/>
-      <c r="W31" s="140"/>
-      <c r="X31" s="140"/>
-      <c r="Y31" s="141"/>
+      <c r="T31" s="129"/>
+      <c r="U31" s="129"/>
+      <c r="V31" s="129"/>
+      <c r="W31" s="129"/>
+      <c r="X31" s="129"/>
+      <c r="Y31" s="130"/>
       <c r="Z31" s="7"/>
     </row>
     <row r="32" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="152"/>
-      <c r="D32" s="152"/>
-      <c r="E32" s="152"/>
-      <c r="F32" s="152"/>
-      <c r="G32" s="152"/>
-      <c r="H32" s="152"/>
-      <c r="I32" s="152"/>
-      <c r="J32" s="155"/>
-      <c r="K32" s="155"/>
-      <c r="L32" s="156"/>
-      <c r="M32" s="154"/>
-      <c r="N32" s="155"/>
-      <c r="O32" s="155"/>
-      <c r="P32" s="155"/>
-      <c r="Q32" s="155"/>
-      <c r="R32" s="155"/>
-      <c r="S32" s="142"/>
-      <c r="T32" s="143"/>
-      <c r="U32" s="143"/>
-      <c r="V32" s="143"/>
-      <c r="W32" s="143"/>
-      <c r="X32" s="143"/>
-      <c r="Y32" s="144"/>
+      <c r="B32" s="248"/>
+      <c r="C32" s="249"/>
+      <c r="D32" s="249"/>
+      <c r="E32" s="249"/>
+      <c r="F32" s="249"/>
+      <c r="G32" s="249"/>
+      <c r="H32" s="249"/>
+      <c r="I32" s="249"/>
+      <c r="J32" s="251"/>
+      <c r="K32" s="251"/>
+      <c r="L32" s="252"/>
+      <c r="M32" s="255"/>
+      <c r="N32" s="251"/>
+      <c r="O32" s="251"/>
+      <c r="P32" s="251"/>
+      <c r="Q32" s="251"/>
+      <c r="R32" s="251"/>
+      <c r="S32" s="131"/>
+      <c r="T32" s="132"/>
+      <c r="U32" s="132"/>
+      <c r="V32" s="132"/>
+      <c r="W32" s="132"/>
+      <c r="X32" s="132"/>
+      <c r="Y32" s="133"/>
       <c r="Z32" s="7"/>
     </row>
     <row r="33" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
-      <c r="B33" s="139" t="s">
+      <c r="B33" s="128" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="140"/>
-      <c r="D33" s="139" t="s">
+      <c r="C33" s="129"/>
+      <c r="D33" s="128" t="s">
         <v>154</v>
       </c>
-      <c r="E33" s="140"/>
-      <c r="F33" s="140"/>
-      <c r="G33" s="140"/>
-      <c r="H33" s="140"/>
-      <c r="I33" s="141"/>
-      <c r="J33" s="140" t="s">
+      <c r="E33" s="129"/>
+      <c r="F33" s="129"/>
+      <c r="G33" s="129"/>
+      <c r="H33" s="129"/>
+      <c r="I33" s="130"/>
+      <c r="J33" s="129" t="s">
         <v>155</v>
       </c>
-      <c r="K33" s="140"/>
-      <c r="L33" s="141"/>
-      <c r="M33" s="139" t="s">
+      <c r="K33" s="129"/>
+      <c r="L33" s="130"/>
+      <c r="M33" s="128" t="s">
         <v>157</v>
       </c>
-      <c r="N33" s="140"/>
-      <c r="O33" s="141"/>
-      <c r="P33" s="139" t="s">
+      <c r="N33" s="129"/>
+      <c r="O33" s="130"/>
+      <c r="P33" s="128" t="s">
         <v>158</v>
       </c>
-      <c r="Q33" s="140"/>
-      <c r="R33" s="140"/>
-      <c r="S33" s="193" t="s">
+      <c r="Q33" s="129"/>
+      <c r="R33" s="129"/>
+      <c r="S33" s="122" t="s">
         <v>227</v>
       </c>
-      <c r="T33" s="194"/>
-      <c r="U33" s="195"/>
-      <c r="V33" s="193" t="s">
+      <c r="T33" s="123"/>
+      <c r="U33" s="124"/>
+      <c r="V33" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="W33" s="194"/>
-      <c r="X33" s="194"/>
-      <c r="Y33" s="195"/>
+      <c r="W33" s="123"/>
+      <c r="X33" s="123"/>
+      <c r="Y33" s="124"/>
       <c r="Z33" s="7"/>
     </row>
     <row r="34" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6"/>
-      <c r="B34" s="145"/>
-      <c r="C34" s="146"/>
-      <c r="D34" s="145"/>
-      <c r="E34" s="146"/>
-      <c r="F34" s="146"/>
-      <c r="G34" s="146"/>
-      <c r="H34" s="146"/>
-      <c r="I34" s="147"/>
-      <c r="J34" s="146"/>
-      <c r="K34" s="146"/>
-      <c r="L34" s="147"/>
-      <c r="M34" s="142"/>
-      <c r="N34" s="143"/>
-      <c r="O34" s="144"/>
-      <c r="P34" s="142"/>
-      <c r="Q34" s="143"/>
-      <c r="R34" s="143"/>
-      <c r="S34" s="196"/>
-      <c r="T34" s="197"/>
-      <c r="U34" s="198"/>
-      <c r="V34" s="196"/>
-      <c r="W34" s="197"/>
-      <c r="X34" s="197"/>
-      <c r="Y34" s="198"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="171"/>
+      <c r="D34" s="170"/>
+      <c r="E34" s="171"/>
+      <c r="F34" s="171"/>
+      <c r="G34" s="171"/>
+      <c r="H34" s="171"/>
+      <c r="I34" s="172"/>
+      <c r="J34" s="171"/>
+      <c r="K34" s="171"/>
+      <c r="L34" s="172"/>
+      <c r="M34" s="131"/>
+      <c r="N34" s="132"/>
+      <c r="O34" s="133"/>
+      <c r="P34" s="131"/>
+      <c r="Q34" s="132"/>
+      <c r="R34" s="132"/>
+      <c r="S34" s="125"/>
+      <c r="T34" s="126"/>
+      <c r="U34" s="127"/>
+      <c r="V34" s="125"/>
+      <c r="W34" s="126"/>
+      <c r="X34" s="126"/>
+      <c r="Y34" s="127"/>
       <c r="Z34" s="7"/>
     </row>
     <row r="35" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
-      <c r="B35" s="293"/>
-      <c r="C35" s="294"/>
-      <c r="D35" s="295"/>
-      <c r="E35" s="296"/>
-      <c r="F35" s="296"/>
-      <c r="G35" s="296"/>
-      <c r="H35" s="296"/>
-      <c r="I35" s="297"/>
-      <c r="J35" s="298"/>
-      <c r="K35" s="296"/>
-      <c r="L35" s="297"/>
-      <c r="M35" s="166"/>
-      <c r="N35" s="166"/>
-      <c r="O35" s="167"/>
-      <c r="P35" s="165"/>
-      <c r="Q35" s="166"/>
-      <c r="R35" s="166"/>
-      <c r="S35" s="284" t="e">
+      <c r="B35" s="143"/>
+      <c r="C35" s="144"/>
+      <c r="D35" s="145"/>
+      <c r="E35" s="146"/>
+      <c r="F35" s="146"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="146"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="148"/>
+      <c r="K35" s="146"/>
+      <c r="L35" s="147"/>
+      <c r="M35" s="152"/>
+      <c r="N35" s="152"/>
+      <c r="O35" s="153"/>
+      <c r="P35" s="158"/>
+      <c r="Q35" s="152"/>
+      <c r="R35" s="152"/>
+      <c r="S35" s="134" t="e">
         <f>SUM($U$13:$V$30)-$W$20</f>
         <v>#REF!</v>
       </c>
-      <c r="T35" s="285"/>
-      <c r="U35" s="286"/>
-      <c r="V35" s="284" t="e">
+      <c r="T35" s="135"/>
+      <c r="U35" s="136"/>
+      <c r="V35" s="134" t="e">
         <f>Purchasing!$K$11</f>
         <v>#REF!</v>
       </c>
-      <c r="W35" s="285"/>
-      <c r="X35" s="285"/>
-      <c r="Y35" s="286"/>
+      <c r="W35" s="135"/>
+      <c r="X35" s="135"/>
+      <c r="Y35" s="136"/>
       <c r="Z35" s="7"/>
     </row>
     <row r="36" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
-      <c r="B36" s="254"/>
-      <c r="C36" s="255"/>
-      <c r="D36" s="208"/>
-      <c r="E36" s="209"/>
-      <c r="F36" s="209"/>
-      <c r="G36" s="209"/>
-      <c r="H36" s="209"/>
-      <c r="I36" s="210"/>
-      <c r="J36" s="211"/>
-      <c r="K36" s="209"/>
-      <c r="L36" s="210"/>
-      <c r="M36" s="169"/>
-      <c r="N36" s="169"/>
-      <c r="O36" s="170"/>
-      <c r="P36" s="168"/>
-      <c r="Q36" s="169"/>
-      <c r="R36" s="169"/>
-      <c r="S36" s="287"/>
-      <c r="T36" s="288"/>
-      <c r="U36" s="289"/>
-      <c r="V36" s="287"/>
-      <c r="W36" s="288"/>
-      <c r="X36" s="288"/>
-      <c r="Y36" s="289"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="117"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="119"/>
+      <c r="F36" s="119"/>
+      <c r="G36" s="119"/>
+      <c r="H36" s="119"/>
+      <c r="I36" s="120"/>
+      <c r="J36" s="121"/>
+      <c r="K36" s="119"/>
+      <c r="L36" s="120"/>
+      <c r="M36" s="154"/>
+      <c r="N36" s="154"/>
+      <c r="O36" s="155"/>
+      <c r="P36" s="159"/>
+      <c r="Q36" s="154"/>
+      <c r="R36" s="154"/>
+      <c r="S36" s="137"/>
+      <c r="T36" s="138"/>
+      <c r="U36" s="139"/>
+      <c r="V36" s="137"/>
+      <c r="W36" s="138"/>
+      <c r="X36" s="138"/>
+      <c r="Y36" s="139"/>
       <c r="Z36" s="7"/>
     </row>
     <row r="37" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
-      <c r="B37" s="254"/>
-      <c r="C37" s="255"/>
-      <c r="D37" s="208"/>
-      <c r="E37" s="209"/>
-      <c r="F37" s="209"/>
-      <c r="G37" s="209"/>
-      <c r="H37" s="209"/>
-      <c r="I37" s="210"/>
-      <c r="J37" s="211"/>
-      <c r="K37" s="209"/>
-      <c r="L37" s="210"/>
-      <c r="M37" s="169"/>
-      <c r="N37" s="169"/>
-      <c r="O37" s="170"/>
-      <c r="P37" s="168"/>
-      <c r="Q37" s="169"/>
-      <c r="R37" s="169"/>
-      <c r="S37" s="287"/>
-      <c r="T37" s="288"/>
-      <c r="U37" s="289"/>
-      <c r="V37" s="287"/>
-      <c r="W37" s="288"/>
-      <c r="X37" s="288"/>
-      <c r="Y37" s="289"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="117"/>
+      <c r="D37" s="118"/>
+      <c r="E37" s="119"/>
+      <c r="F37" s="119"/>
+      <c r="G37" s="119"/>
+      <c r="H37" s="119"/>
+      <c r="I37" s="120"/>
+      <c r="J37" s="121"/>
+      <c r="K37" s="119"/>
+      <c r="L37" s="120"/>
+      <c r="M37" s="154"/>
+      <c r="N37" s="154"/>
+      <c r="O37" s="155"/>
+      <c r="P37" s="159"/>
+      <c r="Q37" s="154"/>
+      <c r="R37" s="154"/>
+      <c r="S37" s="137"/>
+      <c r="T37" s="138"/>
+      <c r="U37" s="139"/>
+      <c r="V37" s="137"/>
+      <c r="W37" s="138"/>
+      <c r="X37" s="138"/>
+      <c r="Y37" s="139"/>
       <c r="Z37" s="7"/>
     </row>
     <row r="38" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6"/>
-      <c r="B38" s="254"/>
-      <c r="C38" s="255"/>
-      <c r="D38" s="208"/>
-      <c r="E38" s="209"/>
-      <c r="F38" s="209"/>
-      <c r="G38" s="209"/>
-      <c r="H38" s="209"/>
-      <c r="I38" s="210"/>
-      <c r="J38" s="211"/>
-      <c r="K38" s="209"/>
-      <c r="L38" s="210"/>
-      <c r="M38" s="169"/>
-      <c r="N38" s="169"/>
-      <c r="O38" s="170"/>
-      <c r="P38" s="168"/>
-      <c r="Q38" s="169"/>
-      <c r="R38" s="169"/>
-      <c r="S38" s="290"/>
-      <c r="T38" s="291"/>
-      <c r="U38" s="292"/>
-      <c r="V38" s="290"/>
-      <c r="W38" s="291"/>
-      <c r="X38" s="291"/>
-      <c r="Y38" s="292"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="117"/>
+      <c r="D38" s="118"/>
+      <c r="E38" s="119"/>
+      <c r="F38" s="119"/>
+      <c r="G38" s="119"/>
+      <c r="H38" s="119"/>
+      <c r="I38" s="120"/>
+      <c r="J38" s="121"/>
+      <c r="K38" s="119"/>
+      <c r="L38" s="120"/>
+      <c r="M38" s="154"/>
+      <c r="N38" s="154"/>
+      <c r="O38" s="155"/>
+      <c r="P38" s="159"/>
+      <c r="Q38" s="154"/>
+      <c r="R38" s="154"/>
+      <c r="S38" s="140"/>
+      <c r="T38" s="141"/>
+      <c r="U38" s="142"/>
+      <c r="V38" s="140"/>
+      <c r="W38" s="141"/>
+      <c r="X38" s="141"/>
+      <c r="Y38" s="142"/>
       <c r="Z38" s="7"/>
     </row>
     <row r="39" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6"/>
-      <c r="B39" s="254"/>
-      <c r="C39" s="255"/>
-      <c r="D39" s="208"/>
-      <c r="E39" s="209"/>
-      <c r="F39" s="209"/>
-      <c r="G39" s="209"/>
-      <c r="H39" s="209"/>
-      <c r="I39" s="210"/>
-      <c r="J39" s="211"/>
-      <c r="K39" s="209"/>
-      <c r="L39" s="210"/>
-      <c r="M39" s="172"/>
-      <c r="N39" s="172"/>
-      <c r="O39" s="173"/>
-      <c r="P39" s="171"/>
-      <c r="Q39" s="172"/>
-      <c r="R39" s="172"/>
-      <c r="S39" s="193" t="s">
+      <c r="B39" s="116"/>
+      <c r="C39" s="117"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="119"/>
+      <c r="F39" s="119"/>
+      <c r="G39" s="119"/>
+      <c r="H39" s="119"/>
+      <c r="I39" s="120"/>
+      <c r="J39" s="121"/>
+      <c r="K39" s="119"/>
+      <c r="L39" s="120"/>
+      <c r="M39" s="156"/>
+      <c r="N39" s="156"/>
+      <c r="O39" s="157"/>
+      <c r="P39" s="160"/>
+      <c r="Q39" s="156"/>
+      <c r="R39" s="156"/>
+      <c r="S39" s="122" t="s">
         <v>228</v>
       </c>
-      <c r="T39" s="194"/>
-      <c r="U39" s="194"/>
-      <c r="V39" s="194"/>
-      <c r="W39" s="194"/>
-      <c r="X39" s="194"/>
-      <c r="Y39" s="195"/>
+      <c r="T39" s="123"/>
+      <c r="U39" s="123"/>
+      <c r="V39" s="123"/>
+      <c r="W39" s="123"/>
+      <c r="X39" s="123"/>
+      <c r="Y39" s="124"/>
       <c r="Z39" s="7"/>
     </row>
     <row r="40" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
-      <c r="B40" s="254"/>
-      <c r="C40" s="255"/>
-      <c r="D40" s="208"/>
-      <c r="E40" s="209"/>
-      <c r="F40" s="209"/>
-      <c r="G40" s="209"/>
-      <c r="H40" s="209"/>
-      <c r="I40" s="210"/>
-      <c r="J40" s="211"/>
-      <c r="K40" s="209"/>
-      <c r="L40" s="210"/>
-      <c r="M40" s="140" t="s">
+      <c r="B40" s="116"/>
+      <c r="C40" s="117"/>
+      <c r="D40" s="118"/>
+      <c r="E40" s="119"/>
+      <c r="F40" s="119"/>
+      <c r="G40" s="119"/>
+      <c r="H40" s="119"/>
+      <c r="I40" s="120"/>
+      <c r="J40" s="121"/>
+      <c r="K40" s="119"/>
+      <c r="L40" s="120"/>
+      <c r="M40" s="129" t="s">
         <v>159</v>
       </c>
-      <c r="N40" s="140"/>
-      <c r="O40" s="141"/>
-      <c r="P40" s="139" t="s">
+      <c r="N40" s="129"/>
+      <c r="O40" s="130"/>
+      <c r="P40" s="128" t="s">
         <v>160</v>
       </c>
-      <c r="Q40" s="140"/>
-      <c r="R40" s="140"/>
-      <c r="S40" s="196"/>
-      <c r="T40" s="197"/>
-      <c r="U40" s="197"/>
-      <c r="V40" s="197"/>
-      <c r="W40" s="197"/>
-      <c r="X40" s="197"/>
-      <c r="Y40" s="198"/>
+      <c r="Q40" s="129"/>
+      <c r="R40" s="129"/>
+      <c r="S40" s="125"/>
+      <c r="T40" s="126"/>
+      <c r="U40" s="126"/>
+      <c r="V40" s="126"/>
+      <c r="W40" s="126"/>
+      <c r="X40" s="126"/>
+      <c r="Y40" s="127"/>
       <c r="Z40" s="7"/>
     </row>
     <row r="41" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6"/>
-      <c r="B41" s="254"/>
-      <c r="C41" s="255"/>
-      <c r="D41" s="208"/>
-      <c r="E41" s="209"/>
-      <c r="F41" s="209"/>
-      <c r="G41" s="209"/>
-      <c r="H41" s="209"/>
-      <c r="I41" s="210"/>
-      <c r="J41" s="211"/>
-      <c r="K41" s="209"/>
-      <c r="L41" s="210"/>
-      <c r="M41" s="143"/>
-      <c r="N41" s="143"/>
-      <c r="O41" s="144"/>
-      <c r="P41" s="142"/>
-      <c r="Q41" s="143"/>
-      <c r="R41" s="144"/>
-      <c r="S41" s="221" t="e">
+      <c r="B41" s="116"/>
+      <c r="C41" s="117"/>
+      <c r="D41" s="118"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="119"/>
+      <c r="G41" s="119"/>
+      <c r="H41" s="119"/>
+      <c r="I41" s="120"/>
+      <c r="J41" s="121"/>
+      <c r="K41" s="119"/>
+      <c r="L41" s="120"/>
+      <c r="M41" s="132"/>
+      <c r="N41" s="132"/>
+      <c r="O41" s="133"/>
+      <c r="P41" s="131"/>
+      <c r="Q41" s="132"/>
+      <c r="R41" s="133"/>
+      <c r="S41" s="201" t="e">
         <f>$V$35-$S$35</f>
         <v>#REF!</v>
       </c>
-      <c r="T41" s="222"/>
-      <c r="U41" s="222"/>
-      <c r="V41" s="222"/>
-      <c r="W41" s="222"/>
-      <c r="X41" s="222"/>
-      <c r="Y41" s="223"/>
+      <c r="T41" s="202"/>
+      <c r="U41" s="202"/>
+      <c r="V41" s="202"/>
+      <c r="W41" s="202"/>
+      <c r="X41" s="202"/>
+      <c r="Y41" s="203"/>
       <c r="Z41" s="7"/>
     </row>
     <row r="42" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
-      <c r="B42" s="254"/>
-      <c r="C42" s="255"/>
-      <c r="D42" s="208"/>
-      <c r="E42" s="209"/>
-      <c r="F42" s="209"/>
-      <c r="G42" s="209"/>
-      <c r="H42" s="209"/>
-      <c r="I42" s="210"/>
-      <c r="J42" s="211"/>
-      <c r="K42" s="209"/>
-      <c r="L42" s="210"/>
-      <c r="M42" s="166"/>
-      <c r="N42" s="166"/>
-      <c r="O42" s="167"/>
-      <c r="P42" s="165"/>
-      <c r="Q42" s="166"/>
-      <c r="R42" s="167"/>
-      <c r="S42" s="224"/>
-      <c r="T42" s="225"/>
-      <c r="U42" s="225"/>
-      <c r="V42" s="225"/>
-      <c r="W42" s="225"/>
-      <c r="X42" s="225"/>
-      <c r="Y42" s="226"/>
+      <c r="B42" s="116"/>
+      <c r="C42" s="117"/>
+      <c r="D42" s="118"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119"/>
+      <c r="G42" s="119"/>
+      <c r="H42" s="119"/>
+      <c r="I42" s="120"/>
+      <c r="J42" s="121"/>
+      <c r="K42" s="119"/>
+      <c r="L42" s="120"/>
+      <c r="M42" s="152"/>
+      <c r="N42" s="152"/>
+      <c r="O42" s="153"/>
+      <c r="P42" s="158"/>
+      <c r="Q42" s="152"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="204"/>
+      <c r="T42" s="205"/>
+      <c r="U42" s="205"/>
+      <c r="V42" s="205"/>
+      <c r="W42" s="205"/>
+      <c r="X42" s="205"/>
+      <c r="Y42" s="206"/>
       <c r="Z42" s="7"/>
     </row>
     <row r="43" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
-      <c r="B43" s="254"/>
-      <c r="C43" s="255"/>
-      <c r="D43" s="208"/>
-      <c r="E43" s="209"/>
-      <c r="F43" s="209"/>
-      <c r="G43" s="209"/>
-      <c r="H43" s="209"/>
-      <c r="I43" s="210"/>
-      <c r="J43" s="211"/>
-      <c r="K43" s="209"/>
-      <c r="L43" s="210"/>
-      <c r="M43" s="169"/>
-      <c r="N43" s="169"/>
-      <c r="O43" s="170"/>
-      <c r="P43" s="168"/>
-      <c r="Q43" s="169"/>
-      <c r="R43" s="170"/>
-      <c r="S43" s="224"/>
-      <c r="T43" s="225"/>
-      <c r="U43" s="225"/>
-      <c r="V43" s="225"/>
-      <c r="W43" s="225"/>
-      <c r="X43" s="225"/>
-      <c r="Y43" s="226"/>
+      <c r="B43" s="116"/>
+      <c r="C43" s="117"/>
+      <c r="D43" s="118"/>
+      <c r="E43" s="119"/>
+      <c r="F43" s="119"/>
+      <c r="G43" s="119"/>
+      <c r="H43" s="119"/>
+      <c r="I43" s="120"/>
+      <c r="J43" s="121"/>
+      <c r="K43" s="119"/>
+      <c r="L43" s="120"/>
+      <c r="M43" s="154"/>
+      <c r="N43" s="154"/>
+      <c r="O43" s="155"/>
+      <c r="P43" s="159"/>
+      <c r="Q43" s="154"/>
+      <c r="R43" s="155"/>
+      <c r="S43" s="204"/>
+      <c r="T43" s="205"/>
+      <c r="U43" s="205"/>
+      <c r="V43" s="205"/>
+      <c r="W43" s="205"/>
+      <c r="X43" s="205"/>
+      <c r="Y43" s="206"/>
       <c r="Z43" s="7"/>
     </row>
     <row r="44" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
-      <c r="B44" s="254"/>
-      <c r="C44" s="255"/>
-      <c r="D44" s="208"/>
-      <c r="E44" s="209"/>
-      <c r="F44" s="209"/>
-      <c r="G44" s="209"/>
-      <c r="H44" s="209"/>
-      <c r="I44" s="210"/>
-      <c r="J44" s="211"/>
-      <c r="K44" s="209"/>
-      <c r="L44" s="210"/>
-      <c r="M44" s="169"/>
-      <c r="N44" s="169"/>
-      <c r="O44" s="170"/>
-      <c r="P44" s="168"/>
-      <c r="Q44" s="169"/>
-      <c r="R44" s="170"/>
-      <c r="S44" s="224"/>
-      <c r="T44" s="225"/>
-      <c r="U44" s="225"/>
-      <c r="V44" s="225"/>
-      <c r="W44" s="225"/>
-      <c r="X44" s="225"/>
-      <c r="Y44" s="226"/>
+      <c r="B44" s="116"/>
+      <c r="C44" s="117"/>
+      <c r="D44" s="118"/>
+      <c r="E44" s="119"/>
+      <c r="F44" s="119"/>
+      <c r="G44" s="119"/>
+      <c r="H44" s="119"/>
+      <c r="I44" s="120"/>
+      <c r="J44" s="121"/>
+      <c r="K44" s="119"/>
+      <c r="L44" s="120"/>
+      <c r="M44" s="154"/>
+      <c r="N44" s="154"/>
+      <c r="O44" s="155"/>
+      <c r="P44" s="159"/>
+      <c r="Q44" s="154"/>
+      <c r="R44" s="155"/>
+      <c r="S44" s="204"/>
+      <c r="T44" s="205"/>
+      <c r="U44" s="205"/>
+      <c r="V44" s="205"/>
+      <c r="W44" s="205"/>
+      <c r="X44" s="205"/>
+      <c r="Y44" s="206"/>
       <c r="Z44" s="7"/>
     </row>
     <row r="45" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
-      <c r="B45" s="254"/>
-      <c r="C45" s="255"/>
-      <c r="D45" s="208"/>
-      <c r="E45" s="209"/>
-      <c r="F45" s="209"/>
-      <c r="G45" s="209"/>
-      <c r="H45" s="209"/>
-      <c r="I45" s="210"/>
-      <c r="J45" s="211"/>
-      <c r="K45" s="209"/>
-      <c r="L45" s="210"/>
-      <c r="M45" s="169"/>
-      <c r="N45" s="169"/>
-      <c r="O45" s="170"/>
-      <c r="P45" s="168"/>
-      <c r="Q45" s="169"/>
-      <c r="R45" s="170"/>
-      <c r="S45" s="224"/>
-      <c r="T45" s="225"/>
-      <c r="U45" s="225"/>
-      <c r="V45" s="225"/>
-      <c r="W45" s="225"/>
-      <c r="X45" s="225"/>
-      <c r="Y45" s="226"/>
+      <c r="B45" s="116"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="119"/>
+      <c r="F45" s="119"/>
+      <c r="G45" s="119"/>
+      <c r="H45" s="119"/>
+      <c r="I45" s="120"/>
+      <c r="J45" s="121"/>
+      <c r="K45" s="119"/>
+      <c r="L45" s="120"/>
+      <c r="M45" s="154"/>
+      <c r="N45" s="154"/>
+      <c r="O45" s="155"/>
+      <c r="P45" s="159"/>
+      <c r="Q45" s="154"/>
+      <c r="R45" s="155"/>
+      <c r="S45" s="204"/>
+      <c r="T45" s="205"/>
+      <c r="U45" s="205"/>
+      <c r="V45" s="205"/>
+      <c r="W45" s="205"/>
+      <c r="X45" s="205"/>
+      <c r="Y45" s="206"/>
       <c r="Z45" s="7"/>
     </row>
     <row r="46" spans="1:26" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
-      <c r="B46" s="256"/>
-      <c r="C46" s="257"/>
-      <c r="D46" s="258"/>
-      <c r="E46" s="259"/>
-      <c r="F46" s="259"/>
-      <c r="G46" s="259"/>
-      <c r="H46" s="259"/>
-      <c r="I46" s="260"/>
-      <c r="J46" s="261"/>
-      <c r="K46" s="259"/>
-      <c r="L46" s="260"/>
-      <c r="M46" s="172"/>
-      <c r="N46" s="172"/>
-      <c r="O46" s="173"/>
-      <c r="P46" s="171"/>
-      <c r="Q46" s="172"/>
-      <c r="R46" s="173"/>
-      <c r="S46" s="227"/>
-      <c r="T46" s="228"/>
-      <c r="U46" s="228"/>
-      <c r="V46" s="228"/>
-      <c r="W46" s="228"/>
-      <c r="X46" s="228"/>
-      <c r="Y46" s="229"/>
+      <c r="B46" s="173"/>
+      <c r="C46" s="174"/>
+      <c r="D46" s="175"/>
+      <c r="E46" s="176"/>
+      <c r="F46" s="176"/>
+      <c r="G46" s="176"/>
+      <c r="H46" s="176"/>
+      <c r="I46" s="177"/>
+      <c r="J46" s="178"/>
+      <c r="K46" s="176"/>
+      <c r="L46" s="177"/>
+      <c r="M46" s="156"/>
+      <c r="N46" s="156"/>
+      <c r="O46" s="157"/>
+      <c r="P46" s="160"/>
+      <c r="Q46" s="156"/>
+      <c r="R46" s="157"/>
+      <c r="S46" s="207"/>
+      <c r="T46" s="208"/>
+      <c r="U46" s="208"/>
+      <c r="V46" s="208"/>
+      <c r="W46" s="208"/>
+      <c r="X46" s="208"/>
+      <c r="Y46" s="209"/>
       <c r="Z46" s="7"/>
     </row>
     <row r="47" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6243,49 +6243,70 @@
     </row>
   </sheetData>
   <mergeCells count="145">
-    <mergeCell ref="U13:V14"/>
-    <mergeCell ref="S15:T16"/>
-    <mergeCell ref="U15:V16"/>
-    <mergeCell ref="W18:Y19"/>
-    <mergeCell ref="S29:T30"/>
-    <mergeCell ref="U29:V30"/>
-    <mergeCell ref="S17:T18"/>
-    <mergeCell ref="U17:V18"/>
-    <mergeCell ref="S19:T20"/>
-    <mergeCell ref="U19:V20"/>
-    <mergeCell ref="W15:Y17"/>
-    <mergeCell ref="S13:T14"/>
-    <mergeCell ref="U21:V22"/>
-    <mergeCell ref="S23:T24"/>
-    <mergeCell ref="U23:V24"/>
-    <mergeCell ref="S25:T26"/>
-    <mergeCell ref="U25:V26"/>
-    <mergeCell ref="S27:T28"/>
-    <mergeCell ref="U27:V28"/>
-    <mergeCell ref="S21:T22"/>
-    <mergeCell ref="W13:Y14"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="S33:U34"/>
-    <mergeCell ref="V33:Y34"/>
-    <mergeCell ref="S31:Y32"/>
-    <mergeCell ref="S35:U38"/>
-    <mergeCell ref="V35:Y38"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:I35"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="M35:O39"/>
-    <mergeCell ref="P35:R39"/>
-    <mergeCell ref="H23:K23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="N22:N25"/>
+    <mergeCell ref="N26:N29"/>
+    <mergeCell ref="Q5:Y7"/>
+    <mergeCell ref="Q3:Y4"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J4:P7"/>
+    <mergeCell ref="B3:D7"/>
+    <mergeCell ref="E3:I7"/>
+    <mergeCell ref="G11:L12"/>
+    <mergeCell ref="B11:F12"/>
+    <mergeCell ref="M11:O12"/>
+    <mergeCell ref="P11:R12"/>
+    <mergeCell ref="S11:Y12"/>
+    <mergeCell ref="S8:Y10"/>
+    <mergeCell ref="M8:R10"/>
+    <mergeCell ref="B8:L10"/>
+    <mergeCell ref="P26:P29"/>
+    <mergeCell ref="Q22:Q25"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="B17:D18"/>
+    <mergeCell ref="B20:D21"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="B30:L32"/>
+    <mergeCell ref="M18:R19"/>
+    <mergeCell ref="M13:O17"/>
+    <mergeCell ref="P13:R17"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="M30:R32"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="E14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="M20:O21"/>
+    <mergeCell ref="P20:R21"/>
+    <mergeCell ref="M26:M29"/>
+    <mergeCell ref="S39:Y40"/>
+    <mergeCell ref="S41:Y46"/>
+    <mergeCell ref="W25:Y30"/>
+    <mergeCell ref="W23:Y24"/>
+    <mergeCell ref="W20:Y22"/>
+    <mergeCell ref="D43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M42:O46"/>
+    <mergeCell ref="M33:O34"/>
+    <mergeCell ref="P33:R34"/>
+    <mergeCell ref="M40:O41"/>
+    <mergeCell ref="P40:R41"/>
     <mergeCell ref="P42:R46"/>
     <mergeCell ref="B33:C34"/>
     <mergeCell ref="D33:I34"/>
@@ -6310,30 +6331,16 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C25:E25"/>
     <mergeCell ref="C26:E26"/>
-    <mergeCell ref="S39:Y40"/>
-    <mergeCell ref="S41:Y46"/>
-    <mergeCell ref="W25:Y30"/>
-    <mergeCell ref="W23:Y24"/>
-    <mergeCell ref="W20:Y22"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M42:O46"/>
-    <mergeCell ref="M33:O34"/>
-    <mergeCell ref="P33:R34"/>
-    <mergeCell ref="M40:O41"/>
-    <mergeCell ref="P40:R41"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="M35:O39"/>
+    <mergeCell ref="P35:R39"/>
+    <mergeCell ref="H23:K23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
     <mergeCell ref="Q26:Q29"/>
     <mergeCell ref="R22:R25"/>
     <mergeCell ref="R26:R29"/>
@@ -6348,46 +6355,39 @@
     <mergeCell ref="O22:O25"/>
     <mergeCell ref="O26:O29"/>
     <mergeCell ref="P22:P25"/>
-    <mergeCell ref="P26:P29"/>
-    <mergeCell ref="Q22:Q25"/>
-    <mergeCell ref="B14:D15"/>
-    <mergeCell ref="B17:D18"/>
-    <mergeCell ref="B20:D21"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="B30:L32"/>
-    <mergeCell ref="M18:R19"/>
-    <mergeCell ref="M13:O17"/>
-    <mergeCell ref="P13:R17"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="M30:R32"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="E14:H15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="M20:O21"/>
-    <mergeCell ref="P20:R21"/>
-    <mergeCell ref="M26:M29"/>
-    <mergeCell ref="N22:N25"/>
-    <mergeCell ref="N26:N29"/>
-    <mergeCell ref="Q5:Y7"/>
-    <mergeCell ref="Q3:Y4"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="J4:P7"/>
-    <mergeCell ref="B3:D7"/>
-    <mergeCell ref="E3:I7"/>
-    <mergeCell ref="G11:L12"/>
-    <mergeCell ref="B11:F12"/>
-    <mergeCell ref="M11:O12"/>
-    <mergeCell ref="P11:R12"/>
-    <mergeCell ref="S11:Y12"/>
-    <mergeCell ref="S8:Y10"/>
-    <mergeCell ref="M8:R10"/>
-    <mergeCell ref="B8:L10"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="S33:U34"/>
+    <mergeCell ref="V33:Y34"/>
+    <mergeCell ref="S31:Y32"/>
+    <mergeCell ref="S35:U38"/>
+    <mergeCell ref="V35:Y38"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:I35"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="U13:V14"/>
+    <mergeCell ref="S15:T16"/>
+    <mergeCell ref="U15:V16"/>
+    <mergeCell ref="W18:Y19"/>
+    <mergeCell ref="S29:T30"/>
+    <mergeCell ref="U29:V30"/>
+    <mergeCell ref="S17:T18"/>
+    <mergeCell ref="U17:V18"/>
+    <mergeCell ref="S19:T20"/>
+    <mergeCell ref="U19:V20"/>
+    <mergeCell ref="W15:Y17"/>
+    <mergeCell ref="S13:T14"/>
+    <mergeCell ref="U21:V22"/>
+    <mergeCell ref="S23:T24"/>
+    <mergeCell ref="U23:V24"/>
+    <mergeCell ref="S25:T26"/>
+    <mergeCell ref="U25:V26"/>
+    <mergeCell ref="S27:T28"/>
+    <mergeCell ref="U27:V28"/>
+    <mergeCell ref="S21:T22"/>
+    <mergeCell ref="W13:Y14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="S41:Y46">
@@ -7816,7 +7816,7 @@
     <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7844,7 +7844,7 @@
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="44">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>34</v>
@@ -8109,42 +8109,42 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="371" t="s">
+      <c r="B21" s="96" t="s">
         <v>356</v>
       </c>
-      <c r="C21" s="371"/>
-      <c r="D21" s="371" t="s">
+      <c r="C21" s="96"/>
+      <c r="D21" s="96" t="s">
         <v>360</v>
       </c>
-      <c r="E21" s="371"/>
+      <c r="E21" s="96"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="371" t="s">
+      <c r="B22" s="96" t="s">
         <v>357</v>
       </c>
-      <c r="C22" s="371"/>
-      <c r="D22" s="371"/>
-      <c r="E22" s="371"/>
+      <c r="C22" s="96"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="371" t="s">
+      <c r="B23" s="96" t="s">
         <v>358</v>
       </c>
-      <c r="C23" s="371"/>
-      <c r="D23" s="371"/>
-      <c r="E23" s="371"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="96"/>
+      <c r="E23" s="96"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B24" s="371" t="s">
+      <c r="B24" s="96" t="s">
         <v>359</v>
       </c>
-      <c r="C24" s="371"/>
-      <c r="D24" s="371"/>
-      <c r="E24" s="371"/>
+      <c r="C24" s="96"/>
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -8294,18 +8294,18 @@
     </row>
     <row r="2" spans="1:19" ht="35.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="78"/>
-      <c r="B2" s="341" t="s">
+      <c r="B2" s="332" t="s">
         <v>260</v>
       </c>
-      <c r="C2" s="342"/>
-      <c r="D2" s="342"/>
-      <c r="E2" s="343"/>
+      <c r="C2" s="333"/>
+      <c r="D2" s="333"/>
+      <c r="E2" s="334"/>
       <c r="F2" s="78"/>
-      <c r="G2" s="341" t="s">
+      <c r="G2" s="332" t="s">
         <v>237</v>
       </c>
-      <c r="H2" s="342"/>
-      <c r="I2" s="343"/>
+      <c r="H2" s="333"/>
+      <c r="I2" s="334"/>
       <c r="J2" s="78"/>
       <c r="K2" s="58" t="s">
         <v>196</v>
@@ -8360,7 +8360,7 @@
       <c r="J3" s="78"/>
       <c r="K3" s="53">
         <f ca="1">TODAY()</f>
-        <v>45175</v>
+        <v>45209</v>
       </c>
       <c r="L3" s="54" t="e">
         <f>BOM!#REF!</f>
@@ -8418,16 +8418,16 @@
         <v>#REF!</v>
       </c>
       <c r="J4" s="78"/>
-      <c r="K4" s="332" t="s">
+      <c r="K4" s="356" t="s">
         <v>263</v>
       </c>
-      <c r="L4" s="333"/>
-      <c r="M4" s="333"/>
-      <c r="N4" s="333"/>
-      <c r="O4" s="333"/>
-      <c r="P4" s="333"/>
-      <c r="Q4" s="333"/>
-      <c r="R4" s="334"/>
+      <c r="L4" s="357"/>
+      <c r="M4" s="357"/>
+      <c r="N4" s="357"/>
+      <c r="O4" s="357"/>
+      <c r="P4" s="357"/>
+      <c r="Q4" s="357"/>
+      <c r="R4" s="358"/>
       <c r="S4" s="78"/>
     </row>
     <row r="5" spans="1:19" ht="32.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8490,16 +8490,16 @@
         <v>#REF!</v>
       </c>
       <c r="J6" s="78"/>
-      <c r="K6" s="335" t="s">
+      <c r="K6" s="359" t="s">
         <v>246</v>
       </c>
-      <c r="L6" s="336"/>
-      <c r="M6" s="336"/>
-      <c r="N6" s="336"/>
-      <c r="O6" s="336"/>
-      <c r="P6" s="336"/>
-      <c r="Q6" s="336"/>
-      <c r="R6" s="337"/>
+      <c r="L6" s="360"/>
+      <c r="M6" s="360"/>
+      <c r="N6" s="360"/>
+      <c r="O6" s="360"/>
+      <c r="P6" s="360"/>
+      <c r="Q6" s="360"/>
+      <c r="R6" s="361"/>
       <c r="S6" s="78"/>
     </row>
     <row r="7" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8526,18 +8526,18 @@
         <v>#REF!</v>
       </c>
       <c r="J7" s="78"/>
-      <c r="K7" s="338" t="s">
+      <c r="K7" s="362" t="s">
         <v>147</v>
       </c>
-      <c r="L7" s="339"/>
-      <c r="M7" s="339"/>
-      <c r="N7" s="339"/>
-      <c r="O7" s="340" t="s">
+      <c r="L7" s="345"/>
+      <c r="M7" s="345"/>
+      <c r="N7" s="345"/>
+      <c r="O7" s="363" t="s">
         <v>247</v>
       </c>
-      <c r="P7" s="339"/>
-      <c r="Q7" s="339"/>
-      <c r="R7" s="317"/>
+      <c r="P7" s="345"/>
+      <c r="Q7" s="345"/>
+      <c r="R7" s="346"/>
       <c r="S7" s="78"/>
     </row>
     <row r="8" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8564,14 +8564,14 @@
         <v>#REF!</v>
       </c>
       <c r="J8" s="78"/>
-      <c r="K8" s="318" t="s">
+      <c r="K8" s="364" t="s">
         <v>248</v>
       </c>
-      <c r="L8" s="319"/>
-      <c r="M8" s="324" t="s">
+      <c r="L8" s="365"/>
+      <c r="M8" s="366" t="s">
         <v>249</v>
       </c>
-      <c r="N8" s="324"/>
+      <c r="N8" s="366"/>
       <c r="O8" s="62" t="s">
         <v>214</v>
       </c>
@@ -8612,21 +8612,21 @@
         <v>#REF!</v>
       </c>
       <c r="J9" s="78"/>
-      <c r="K9" s="320">
+      <c r="K9" s="351">
         <v>86.93</v>
       </c>
-      <c r="L9" s="321"/>
-      <c r="M9" s="322" t="e">
+      <c r="L9" s="341"/>
+      <c r="M9" s="342" t="e">
         <f>$M$11/Overview!$E$17</f>
         <v>#REF!</v>
       </c>
-      <c r="N9" s="322"/>
-      <c r="O9" s="315" t="s">
+      <c r="N9" s="342"/>
+      <c r="O9" s="343" t="s">
         <v>254</v>
       </c>
-      <c r="P9" s="316"/>
-      <c r="Q9" s="316"/>
-      <c r="R9" s="317"/>
+      <c r="P9" s="344"/>
+      <c r="Q9" s="344"/>
+      <c r="R9" s="346"/>
       <c r="S9" s="78"/>
     </row>
     <row r="10" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8658,19 +8658,19 @@
       <c r="K10" s="325" t="s">
         <v>250</v>
       </c>
-      <c r="L10" s="326"/>
-      <c r="M10" s="324" t="s">
+      <c r="L10" s="368"/>
+      <c r="M10" s="366" t="s">
         <v>251</v>
       </c>
-      <c r="N10" s="324"/>
-      <c r="O10" s="318" t="s">
+      <c r="N10" s="366"/>
+      <c r="O10" s="364" t="s">
         <v>255</v>
       </c>
-      <c r="P10" s="319"/>
-      <c r="Q10" s="324" t="s">
+      <c r="P10" s="365"/>
+      <c r="Q10" s="366" t="s">
         <v>256</v>
       </c>
-      <c r="R10" s="328"/>
+      <c r="R10" s="369"/>
       <c r="S10" s="78"/>
     </row>
     <row r="11" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8699,26 +8699,26 @@
         <v>#REF!</v>
       </c>
       <c r="J11" s="78"/>
-      <c r="K11" s="327" t="e">
+      <c r="K11" s="340" t="e">
         <f>$K$9*Overview!$E$17</f>
         <v>#REF!</v>
       </c>
-      <c r="L11" s="321"/>
-      <c r="M11" s="322" t="e">
+      <c r="L11" s="341"/>
+      <c r="M11" s="342" t="e">
         <f>Overview!$S$35</f>
         <v>#REF!</v>
       </c>
-      <c r="N11" s="322"/>
-      <c r="O11" s="329" t="str">
+      <c r="N11" s="342"/>
+      <c r="O11" s="370" t="str">
         <f>Overview!$W$25</f>
         <v>0</v>
       </c>
-      <c r="P11" s="330"/>
-      <c r="Q11" s="322">
+      <c r="P11" s="371"/>
+      <c r="Q11" s="342">
         <f>Overview!$W$15</f>
         <v>0</v>
       </c>
-      <c r="R11" s="331"/>
+      <c r="R11" s="352"/>
       <c r="S11" s="78"/>
     </row>
     <row r="12" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8745,20 +8745,20 @@
         <v>#REF!</v>
       </c>
       <c r="J12" s="78"/>
-      <c r="K12" s="323" t="s">
+      <c r="K12" s="367" t="s">
         <v>252</v>
       </c>
-      <c r="L12" s="319"/>
-      <c r="M12" s="324" t="s">
+      <c r="L12" s="365"/>
+      <c r="M12" s="366" t="s">
         <v>225</v>
       </c>
-      <c r="N12" s="324"/>
-      <c r="O12" s="315" t="s">
+      <c r="N12" s="366"/>
+      <c r="O12" s="343" t="s">
         <v>239</v>
       </c>
-      <c r="P12" s="316"/>
-      <c r="Q12" s="339"/>
-      <c r="R12" s="317"/>
+      <c r="P12" s="344"/>
+      <c r="Q12" s="345"/>
+      <c r="R12" s="346"/>
       <c r="S12" s="78"/>
     </row>
     <row r="13" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8785,21 +8785,21 @@
         <v>#REF!</v>
       </c>
       <c r="J13" s="78"/>
-      <c r="K13" s="327">
+      <c r="K13" s="340">
         <f>SUM(C4:D15)-$M$13</f>
         <v>1695.77</v>
       </c>
-      <c r="L13" s="321"/>
-      <c r="M13" s="322"/>
-      <c r="N13" s="322"/>
-      <c r="O13" s="351" t="s">
+      <c r="L13" s="341"/>
+      <c r="M13" s="342"/>
+      <c r="N13" s="342"/>
+      <c r="O13" s="347" t="s">
         <v>257</v>
       </c>
-      <c r="P13" s="352"/>
-      <c r="Q13" s="353" t="s">
+      <c r="P13" s="348"/>
+      <c r="Q13" s="349" t="s">
         <v>258</v>
       </c>
-      <c r="R13" s="354"/>
+      <c r="R13" s="350"/>
       <c r="S13" s="78"/>
     </row>
     <row r="14" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8829,19 +8829,19 @@
       <c r="K14" s="325" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="365"/>
-      <c r="M14" s="366"/>
-      <c r="N14" s="366"/>
-      <c r="O14" s="320" t="e">
+      <c r="L14" s="326"/>
+      <c r="M14" s="327"/>
+      <c r="N14" s="327"/>
+      <c r="O14" s="351" t="e">
         <f>$K$9-$M$9</f>
         <v>#REF!</v>
       </c>
-      <c r="P14" s="321"/>
-      <c r="Q14" s="322" t="e">
+      <c r="P14" s="341"/>
+      <c r="Q14" s="342" t="e">
         <f>$K$11-$M$11</f>
         <v>#REF!</v>
       </c>
-      <c r="R14" s="331"/>
+      <c r="R14" s="352"/>
       <c r="S14" s="78"/>
     </row>
     <row r="15" spans="1:19" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8863,47 +8863,47 @@
       <c r="H15" s="70"/>
       <c r="I15" s="74"/>
       <c r="J15" s="78"/>
-      <c r="K15" s="367" t="e">
+      <c r="K15" s="328" t="e">
         <f>IF(SUM($C$4:$D$14)=0,"No Baskets",$K$11-$K$13)</f>
         <v>#REF!</v>
       </c>
-      <c r="L15" s="368"/>
-      <c r="M15" s="368"/>
-      <c r="N15" s="368"/>
-      <c r="O15" s="358" t="s">
+      <c r="L15" s="329"/>
+      <c r="M15" s="329"/>
+      <c r="N15" s="329"/>
+      <c r="O15" s="318" t="s">
         <v>259</v>
       </c>
-      <c r="P15" s="359"/>
-      <c r="Q15" s="360"/>
-      <c r="R15" s="361"/>
+      <c r="P15" s="319"/>
+      <c r="Q15" s="320"/>
+      <c r="R15" s="321"/>
       <c r="S15" s="78"/>
     </row>
     <row r="16" spans="1:19" ht="42.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="78"/>
-      <c r="B16" s="355" t="s">
+      <c r="B16" s="353" t="s">
         <v>261</v>
       </c>
-      <c r="C16" s="356"/>
-      <c r="D16" s="356"/>
-      <c r="E16" s="357"/>
+      <c r="C16" s="354"/>
+      <c r="D16" s="354"/>
+      <c r="E16" s="355"/>
       <c r="F16" s="78"/>
-      <c r="G16" s="355" t="s">
+      <c r="G16" s="353" t="s">
         <v>262</v>
       </c>
-      <c r="H16" s="356"/>
-      <c r="I16" s="357"/>
+      <c r="H16" s="354"/>
+      <c r="I16" s="355"/>
       <c r="J16" s="78"/>
-      <c r="K16" s="369"/>
-      <c r="L16" s="370"/>
-      <c r="M16" s="370"/>
-      <c r="N16" s="370"/>
-      <c r="O16" s="362" t="e">
+      <c r="K16" s="330"/>
+      <c r="L16" s="331"/>
+      <c r="M16" s="331"/>
+      <c r="N16" s="331"/>
+      <c r="O16" s="322" t="e">
         <f>$M$11-$K$13</f>
         <v>#REF!</v>
       </c>
-      <c r="P16" s="363"/>
-      <c r="Q16" s="363"/>
-      <c r="R16" s="364"/>
+      <c r="P16" s="323"/>
+      <c r="Q16" s="323"/>
+      <c r="R16" s="324"/>
       <c r="S16" s="78"/>
     </row>
     <row r="17" spans="1:19" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -8917,15 +8917,15 @@
       <c r="H17" s="78"/>
       <c r="I17" s="78"/>
       <c r="J17" s="78"/>
-      <c r="K17" s="349" t="s">
+      <c r="K17" s="316" t="s">
         <v>265</v>
       </c>
-      <c r="L17" s="350"/>
-      <c r="M17" s="349" t="e">
+      <c r="L17" s="317"/>
+      <c r="M17" s="316" t="e">
         <f t="shared" ref="M17" si="2">IF($K$15="No Baskets","No Baskets",IF($K$15&gt;0,"N/A","Needs approval!"))</f>
         <v>#REF!</v>
       </c>
-      <c r="N17" s="350"/>
+      <c r="N17" s="317"/>
       <c r="O17" s="78"/>
       <c r="P17" s="78"/>
       <c r="Q17" s="78"/>
@@ -8937,32 +8937,32 @@
       <c r="B18" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="344" t="e">
+      <c r="C18" s="335" t="e">
         <f>Overview!$E$3</f>
         <v>#REF!</v>
       </c>
-      <c r="D18" s="344"/>
-      <c r="E18" s="345" t="e">
+      <c r="D18" s="335"/>
+      <c r="E18" s="336" t="e">
         <f>Overview!$J$4</f>
         <v>#REF!</v>
       </c>
-      <c r="F18" s="346"/>
-      <c r="G18" s="346"/>
-      <c r="H18" s="346"/>
-      <c r="I18" s="346"/>
-      <c r="J18" s="346"/>
-      <c r="K18" s="345" t="e">
+      <c r="F18" s="337"/>
+      <c r="G18" s="337"/>
+      <c r="H18" s="337"/>
+      <c r="I18" s="337"/>
+      <c r="J18" s="337"/>
+      <c r="K18" s="336" t="e">
         <f>Overview!$E$20</f>
         <v>#REF!</v>
       </c>
-      <c r="L18" s="346"/>
-      <c r="M18" s="346"/>
-      <c r="N18" s="346"/>
-      <c r="O18" s="346"/>
-      <c r="P18" s="347" t="s">
+      <c r="L18" s="337"/>
+      <c r="M18" s="337"/>
+      <c r="N18" s="337"/>
+      <c r="O18" s="337"/>
+      <c r="P18" s="338" t="s">
         <v>150</v>
       </c>
-      <c r="Q18" s="348"/>
+      <c r="Q18" s="339"/>
       <c r="R18" s="52" t="e">
         <f>Overview!$E$17</f>
         <v>#REF!</v>
@@ -8992,11 +8992,25 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N16"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="K6:R6"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="E18:J18"/>
@@ -9013,25 +9027,11 @@
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B16:E16"/>
     <mergeCell ref="G16:I16"/>
-    <mergeCell ref="K4:R4"/>
-    <mergeCell ref="K6:R6"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N16"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:E15">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">

</xml_diff>